<commit_message>
clean code ruleset complete + beginning quality index ruleset
</commit_message>
<xml_diff>
--- a/files/Rule-Sets.xlsx
+++ b/files/Rule-Sets.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="120" windowWidth="20868" windowHeight="7416"/>
+    <workbookView xWindow="672" yWindow="120" windowWidth="20868" windowHeight="7416" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Elements of Java Style" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Clean Code" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="Ruleset_Clean_Code" localSheetId="1">'Clean Code'!$A$1:$F$67</definedName>
     <definedName name="Ruleset_Elements_Of_Java_Style" localSheetId="0">'Elements of Java Style'!$A$1:$F$109</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +21,19 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Ruleset_Elements-Of-Java-Style" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="1" name="Ruleset_Clean-Code" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\Develop\Diplom\git_repo\files\Ruleset_Clean-Code.csv" decimal="," thousands="." tab="0" semicolon="1" qualifier="none">
+      <textFields count="6">
+        <textField type="text"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="Ruleset_Elements-Of-Java-Style" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\jnru\Desktop\Ruleset_Elements-Of-Java-Style.csv" decimal="," thousands="." tab="0" semicolon="1" qualifier="none">
       <textFields count="6">
         <textField type="text"/>
@@ -36,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="598">
   <si>
     <t>ID</t>
   </si>
@@ -1164,6 +1177,672 @@
   </si>
   <si>
     <t>Structure, Coding</t>
+  </si>
+  <si>
+    <t>CLC-C01</t>
+  </si>
+  <si>
+    <t>Kommentare</t>
+  </si>
+  <si>
+    <t>Ungeeignete Information</t>
+  </si>
+  <si>
+    <t>Keine ungeeigneten Informationen in Kommentaren (z.B. Versionen in SVN)</t>
+  </si>
+  <si>
+    <t>CLC-C02</t>
+  </si>
+  <si>
+    <t>Überholte Kommentare</t>
+  </si>
+  <si>
+    <t>Keine veralteten Kommentare im Code belassen</t>
+  </si>
+  <si>
+    <t>CLC-C03</t>
+  </si>
+  <si>
+    <t>Redundante Kommentare</t>
+  </si>
+  <si>
+    <t>Keine Kommentare mit Informationen die unmittelbar aus dem Code hervorgehen</t>
+  </si>
+  <si>
+    <t>CLC-C04</t>
+  </si>
+  <si>
+    <t>Schlecht geschriebene Kommentare</t>
+  </si>
+  <si>
+    <t>Kommentare gut verständlich und präzise schreiben</t>
+  </si>
+  <si>
+    <t>CLC-C05</t>
+  </si>
+  <si>
+    <t>Auskommentierter Code</t>
+  </si>
+  <si>
+    <t>Code nicht auskommentieren</t>
+  </si>
+  <si>
+    <t>CLC-E01</t>
+  </si>
+  <si>
+    <t>Umgebung</t>
+  </si>
+  <si>
+    <t>Ein Build erfordert mehr als einen Schritt</t>
+  </si>
+  <si>
+    <t>Der Build sollte durch eine einzelne triviale Operation erfolgen</t>
+  </si>
+  <si>
+    <t>CLC-E02</t>
+  </si>
+  <si>
+    <t>Tests erfordern mehr als einen Schritt</t>
+  </si>
+  <si>
+    <t>Alle Tests sollten sich mit Hilfe einer einzelnen trivialen Operation ausführen lassen</t>
+  </si>
+  <si>
+    <t>Tests, Coding</t>
+  </si>
+  <si>
+    <t>CLC-F01</t>
+  </si>
+  <si>
+    <t>Funktionen</t>
+  </si>
+  <si>
+    <t>Zu viele Argumente</t>
+  </si>
+  <si>
+    <t>So wenig Methodenparameter wie möglich, maximal 3</t>
+  </si>
+  <si>
+    <t>CLC-F02</t>
+  </si>
+  <si>
+    <t>Output-Argumente</t>
+  </si>
+  <si>
+    <t>Keine Methodenparameter überschreiben (als Ergebnisvariable benutzen)</t>
+  </si>
+  <si>
+    <t>Methods, Variables</t>
+  </si>
+  <si>
+    <t>CLC-F03</t>
+  </si>
+  <si>
+    <t>Flag-Argumente</t>
+  </si>
+  <si>
+    <t>Keine Booealschen Methodenparameter</t>
+  </si>
+  <si>
+    <t>CLC-F04</t>
+  </si>
+  <si>
+    <t>Tote Funktionen</t>
+  </si>
+  <si>
+    <t>Nicht verwendete Methoden entfernen</t>
+  </si>
+  <si>
+    <t>Methods, Unused</t>
+  </si>
+  <si>
+    <t>CLC-G01</t>
+  </si>
+  <si>
+    <t>Allgemein</t>
+  </si>
+  <si>
+    <t>Mehrere Sprachen in einer Quelldatei</t>
+  </si>
+  <si>
+    <t>So wenig Sprachen (Programmiersprachen und natürliche Sprachen) wie möglich in einer Datei verwenden</t>
+  </si>
+  <si>
+    <t>CLC-G02</t>
+  </si>
+  <si>
+    <t>Offensichtliches Verhalten ist nicht implementiert</t>
+  </si>
+  <si>
+    <t>Methoden so implementieren wie man es erwarten würde (entsprechende Namen)</t>
+  </si>
+  <si>
+    <t>CLC-G03</t>
+  </si>
+  <si>
+    <t>Falsches Verhalten an den Grenzen</t>
+  </si>
+  <si>
+    <t>Alle Grenzwerte und Sonderfälle für Parameter testen</t>
+  </si>
+  <si>
+    <t>Methods, Tests</t>
+  </si>
+  <si>
+    <t>CLC-G04</t>
+  </si>
+  <si>
+    <t>Übergangene Sicherungen</t>
+  </si>
+  <si>
+    <t>Fehlschlagende Tests, Exceptions und Warnungen nicht ignorieren</t>
+  </si>
+  <si>
+    <t>Tests, Exceptions</t>
+  </si>
+  <si>
+    <t>CLC-G05</t>
+  </si>
+  <si>
+    <t>Duplizierung</t>
+  </si>
+  <si>
+    <t>Keine Code-Duplizierung - Auslagerung in Methoden</t>
+  </si>
+  <si>
+    <t>CLC-G06</t>
+  </si>
+  <si>
+    <t>Auf der falschen Abstraktionsebene codieren</t>
+  </si>
+  <si>
+    <t>In jeder Methode / Klasse / Interface nur eine Abstraktionsebene betrachten</t>
+  </si>
+  <si>
+    <t>Classes, Methods</t>
+  </si>
+  <si>
+    <t>CLC-G07</t>
+  </si>
+  <si>
+    <t>Basisklasse hängt von abgeleiteten klassen ab</t>
+  </si>
+  <si>
+    <t>Keine Referenzen auf erbende Klassen in Oberklasse</t>
+  </si>
+  <si>
+    <t>CLC-G08</t>
+  </si>
+  <si>
+    <t>Zu viele Informationen</t>
+  </si>
+  <si>
+    <t>Signaturen von Klassen(public Methoden) und Methoden(Parameter) klein halten</t>
+  </si>
+  <si>
+    <t>CLC-G09</t>
+  </si>
+  <si>
+    <t>Toter Code</t>
+  </si>
+  <si>
+    <t>Nicht verwendeten Code entfernen</t>
+  </si>
+  <si>
+    <t>Unused</t>
+  </si>
+  <si>
+    <t>CLC-G10</t>
+  </si>
+  <si>
+    <t>Vertikale Trennung</t>
+  </si>
+  <si>
+    <t>Lokale Variablen über erster Verwendung und private Methoden direkt unter erster Verwendung deklarieren</t>
+  </si>
+  <si>
+    <t>CLC-G11</t>
+  </si>
+  <si>
+    <t>Inkonsistenz</t>
+  </si>
+  <si>
+    <t>Ähnliche Klassen/Methoden/Variablennamen für gleichartige Konstrukte</t>
+  </si>
+  <si>
+    <t>CLC-G12</t>
+  </si>
+  <si>
+    <t>Müll</t>
+  </si>
+  <si>
+    <t>Alles überflüssige Entfernen</t>
+  </si>
+  <si>
+    <t>CLC-G13</t>
+  </si>
+  <si>
+    <t>Künstliche Kopplung</t>
+  </si>
+  <si>
+    <t>Allgemeine Konstrukte nicht in speziellen Klassen deklarieren</t>
+  </si>
+  <si>
+    <t>Enums, Classes</t>
+  </si>
+  <si>
+    <t>CLC-G14</t>
+  </si>
+  <si>
+    <t>Funktionsneid</t>
+  </si>
+  <si>
+    <t>Möglichst nur die Variablen der eigenen Klasse manipulieren</t>
+  </si>
+  <si>
+    <t>Variables, Classes</t>
+  </si>
+  <si>
+    <t>CLC-G15</t>
+  </si>
+  <si>
+    <t>Selektor-Argumente</t>
+  </si>
+  <si>
+    <t>CLC-G16</t>
+  </si>
+  <si>
+    <t>Verdeckte Absicht</t>
+  </si>
+  <si>
+    <t>Absicht des Codes deutlich machen(sprechende Namen, keine Abkürzungen und magischen Zahlen)</t>
+  </si>
+  <si>
+    <t>CLC-G17</t>
+  </si>
+  <si>
+    <t>Falsche zuständigkeit</t>
+  </si>
+  <si>
+    <t>Methoden und Variablen an der erwarteten Stelle deklarieren</t>
+  </si>
+  <si>
+    <t>CLC-G18</t>
+  </si>
+  <si>
+    <t>Fälschlich als statisch deklarierte Methoden</t>
+  </si>
+  <si>
+    <t>Keine polymorphen Methoden als static deklarieren</t>
+  </si>
+  <si>
+    <t>CLC-G19</t>
+  </si>
+  <si>
+    <t>Aussagekräftige Variablen verwenden</t>
+  </si>
+  <si>
+    <t>Zwischenergebnisse in gut benannten Variablen ablegen</t>
+  </si>
+  <si>
+    <t>CLC-G20</t>
+  </si>
+  <si>
+    <t>Funktionsname sollte die Aktion ausdrücken</t>
+  </si>
+  <si>
+    <t>Sprechende Namen für Methoden</t>
+  </si>
+  <si>
+    <t>CLC-G21</t>
+  </si>
+  <si>
+    <t>Den Algorithmus verstehen</t>
+  </si>
+  <si>
+    <t>Vor der Implementierung den Algorithmus wirklich verstehen</t>
+  </si>
+  <si>
+    <t>CLC-G22</t>
+  </si>
+  <si>
+    <t>Logische Abhängigkeiten in physische umwandeln</t>
+  </si>
+  <si>
+    <t>Implizite Abhängigkeiten explizit abbilden</t>
+  </si>
+  <si>
+    <t>CLC-G23</t>
+  </si>
+  <si>
+    <t>Polymorphismus statt If/Else oder Switch/Case verwenden</t>
+  </si>
+  <si>
+    <t>Methoden in Unterklassen polymorph Überschreiben anstatt switch-Anweisungen oder If/Else-Ketten</t>
+  </si>
+  <si>
+    <t>Conditionals, Inheritance</t>
+  </si>
+  <si>
+    <t>CLC-G24</t>
+  </si>
+  <si>
+    <t>Konventionen beachten</t>
+  </si>
+  <si>
+    <t>Zuvor festgelegte Coding Conventions befolgen</t>
+  </si>
+  <si>
+    <t>Style, Coding</t>
+  </si>
+  <si>
+    <t>CLC-G25</t>
+  </si>
+  <si>
+    <t>Magische Zahlen durch benannte Konstanten ersetzen</t>
+  </si>
+  <si>
+    <t>Keine magischen Zahlen verwenden</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t>CLC-G26</t>
+  </si>
+  <si>
+    <t>Präzise sein</t>
+  </si>
+  <si>
+    <t>Präzise Entscheidungen treffen und implementieren:oding</t>
+  </si>
+  <si>
+    <t>CLC-G27</t>
+  </si>
+  <si>
+    <t>Struktur ist wichtiger als Konvention</t>
+  </si>
+  <si>
+    <t>Design durch Struktur umsetzen, nicht durch konvention</t>
+  </si>
+  <si>
+    <t>Structure, Inheritance</t>
+  </si>
+  <si>
+    <t>CLC-G28</t>
+  </si>
+  <si>
+    <t>Bedingungen einkapseln</t>
+  </si>
+  <si>
+    <t>Nicht triviale Bedingungen in Methoden mit sprechendem Namen einkapseln</t>
+  </si>
+  <si>
+    <t>Conditionals, Naming</t>
+  </si>
+  <si>
+    <t>CLC-G29</t>
+  </si>
+  <si>
+    <t>Negative Bedingungen vermeiden</t>
+  </si>
+  <si>
+    <t>Möglichst keine Negierung von Bedingungen</t>
+  </si>
+  <si>
+    <t>CLC-G30</t>
+  </si>
+  <si>
+    <t>Eine Aufgabe pro Funktion!</t>
+  </si>
+  <si>
+    <t>Methoden möglichst kurz - nur eine Aufgabe</t>
+  </si>
+  <si>
+    <t>CLC-G31</t>
+  </si>
+  <si>
+    <t>Verborgene zeitliche Kopplung</t>
+  </si>
+  <si>
+    <t>Erforderliche Reihenfolge von Methoden erzwingen (Parameter / private + aufrufende Methode)</t>
+  </si>
+  <si>
+    <t>CLC-G32</t>
+  </si>
+  <si>
+    <t>Keine Willkür</t>
+  </si>
+  <si>
+    <t>Konsistente begründete Struktur und Benennung</t>
+  </si>
+  <si>
+    <t>CLC-G33</t>
+  </si>
+  <si>
+    <t>Grenzbedingung einkapseln</t>
+  </si>
+  <si>
+    <t>Inkrement / Dekrement einmalig in Variable ablegen</t>
+  </si>
+  <si>
+    <t>CLC-G34</t>
+  </si>
+  <si>
+    <t>In Funktionen nur eine Abstraktionsebene tiefer gehen</t>
+  </si>
+  <si>
+    <t>In jeder Methode nur eine Abstraktionsebene betrachten</t>
+  </si>
+  <si>
+    <t>CLC-G35</t>
+  </si>
+  <si>
+    <t>Konfigurierbare Daten hoch ansiedeln</t>
+  </si>
+  <si>
+    <t>Konfigurationswerte auf hoher Abstraktionsebene definieren</t>
+  </si>
+  <si>
+    <t>Variables, Constants</t>
+  </si>
+  <si>
+    <t>CLC-G36</t>
+  </si>
+  <si>
+    <t>Transitive Navigation vermeiden</t>
+  </si>
+  <si>
+    <t>Konstrukte der Form object.methodCall().otherMethodCall() vermeiden</t>
+  </si>
+  <si>
+    <t>CLC-J01</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Lange Importlisten durch Platzhalter vermeiden</t>
+  </si>
+  <si>
+    <t>Wildcard-Import verwenden bei mehr als 2 Klassen aus Package</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>CLC-J02</t>
+  </si>
+  <si>
+    <t>Keine Konstanten Vererben</t>
+  </si>
+  <si>
+    <t>Statischer Import für Konstanten anstatt Vererbung</t>
+  </si>
+  <si>
+    <t>Constants, Inheritance</t>
+  </si>
+  <si>
+    <t>CLC-J03</t>
+  </si>
+  <si>
+    <t>Konstanten im Gegensatz zu Enums</t>
+  </si>
+  <si>
+    <t>Enums anstatt final static int variablen benutzen</t>
+  </si>
+  <si>
+    <t>Enums</t>
+  </si>
+  <si>
+    <t>CLC-N01</t>
+  </si>
+  <si>
+    <t>Namen</t>
+  </si>
+  <si>
+    <t>Deskriptive Namen wählen</t>
+  </si>
+  <si>
+    <t>Alles mit sprechenden Namen deklarieren</t>
+  </si>
+  <si>
+    <t>CLC-N02</t>
+  </si>
+  <si>
+    <t>Namen sollten der Abstraktionsebene entsprechen</t>
+  </si>
+  <si>
+    <t>Benamung nach Sonderfällen vermeiden</t>
+  </si>
+  <si>
+    <t>CLC-N03</t>
+  </si>
+  <si>
+    <t>Möglichst Standardnomenklatur verwenden</t>
+  </si>
+  <si>
+    <t>Übliche Namenskonventionen befolgen - Je allgemeingültiger desto besser</t>
+  </si>
+  <si>
+    <t>CLC-N04</t>
+  </si>
+  <si>
+    <t>Eindeutige Namen</t>
+  </si>
+  <si>
+    <t>Namen sollten Zweck des Konstrukts eindeutig beschreiben</t>
+  </si>
+  <si>
+    <t>CLC-N05</t>
+  </si>
+  <si>
+    <t>Lange Namen für große Geltungsbereiche</t>
+  </si>
+  <si>
+    <t>Wegwerfvariablen mit kurzem Geltungsbereich dürfen kurze Namen haben</t>
+  </si>
+  <si>
+    <t>CLC-N06</t>
+  </si>
+  <si>
+    <t>Codierungen vermeiden</t>
+  </si>
+  <si>
+    <t>Keine Typ- oder Geltungsbereich-Codes in Namen einbetten</t>
+  </si>
+  <si>
+    <t>CLC-N07</t>
+  </si>
+  <si>
+    <t>Namen sollten Nebeneffekte beschreiben</t>
+  </si>
+  <si>
+    <t>Alle Funktionen eines Konstrukts im Namen ausdrücken</t>
+  </si>
+  <si>
+    <t>CLC-T01</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Unzureichende Tests</t>
+  </si>
+  <si>
+    <t>Alle Bedingungen mit Tests abdecken und Berechnungen validieren</t>
+  </si>
+  <si>
+    <t>CLC-T02</t>
+  </si>
+  <si>
+    <t>Ein Coverage-Tool verwenden</t>
+  </si>
+  <si>
+    <t>testabdeckung automatisiert ermitteln</t>
+  </si>
+  <si>
+    <t>CLC-T03</t>
+  </si>
+  <si>
+    <t>Triviale Tests nicht überspringen</t>
+  </si>
+  <si>
+    <t>Auch triviale Tests schreiben</t>
+  </si>
+  <si>
+    <t>CLC-T04</t>
+  </si>
+  <si>
+    <t>Ein ignorierter Test zeigt eine Mehrdeutigkeit auf</t>
+  </si>
+  <si>
+    <t>Tests mit (noch) unklarem Ergebnis ignorieren</t>
+  </si>
+  <si>
+    <t>CLC-T05</t>
+  </si>
+  <si>
+    <t>Grenzbedingungen testen</t>
+  </si>
+  <si>
+    <t>Alle Grenzwerte und Sonderfälle mit Tests abdecken</t>
+  </si>
+  <si>
+    <t>CLC-T06</t>
+  </si>
+  <si>
+    <t>Bei Bugs die Nachbarschaft gründlich testen</t>
+  </si>
+  <si>
+    <t>Tritt ein fehler auf, weitere Tests für betroffene Funktion durchführen</t>
+  </si>
+  <si>
+    <t>CLC-T07</t>
+  </si>
+  <si>
+    <t>Das Muster des Scheiterns zur Diagnose nutzen</t>
+  </si>
+  <si>
+    <t>Muster der fehlschlagenden Tests als Hinweis auf Problem nutzen</t>
+  </si>
+  <si>
+    <t>CLC-T08</t>
+  </si>
+  <si>
+    <t>Hinweise durch Coverage-Patterns</t>
+  </si>
+  <si>
+    <t>Muster des durch Tests abgedeckten Codes als Hinweis auf Problem nutzen</t>
+  </si>
+  <si>
+    <t>CLC-T09</t>
+  </si>
+  <si>
+    <t>Tests sollten schnell sein</t>
+  </si>
+  <si>
+    <t>Tests bestmöglich beschleunigen</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1896,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Ruleset_Elements-Of-Java-Style" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Ruleset_Elements-Of-Java-Style" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Ruleset_Clean-Code" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1509,7 +2192,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3708,12 +4393,1357 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D2" t="s">
+        <v>379</v>
+      </c>
+      <c r="E2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C3" t="s">
+        <v>381</v>
+      </c>
+      <c r="D3" t="s">
+        <v>382</v>
+      </c>
+      <c r="E3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C4" t="s">
+        <v>384</v>
+      </c>
+      <c r="D4" t="s">
+        <v>385</v>
+      </c>
+      <c r="E4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B5" t="s">
+        <v>377</v>
+      </c>
+      <c r="C5" t="s">
+        <v>387</v>
+      </c>
+      <c r="D5" t="s">
+        <v>388</v>
+      </c>
+      <c r="E5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B6" t="s">
+        <v>377</v>
+      </c>
+      <c r="C6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6" t="s">
+        <v>391</v>
+      </c>
+      <c r="E6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C7" t="s">
+        <v>394</v>
+      </c>
+      <c r="D7" t="s">
+        <v>395</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C8" t="s">
+        <v>397</v>
+      </c>
+      <c r="D8" t="s">
+        <v>398</v>
+      </c>
+      <c r="E8" t="s">
+        <v>399</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B9" t="s">
+        <v>401</v>
+      </c>
+      <c r="C9" t="s">
+        <v>402</v>
+      </c>
+      <c r="D9" t="s">
+        <v>403</v>
+      </c>
+      <c r="E9" t="s">
+        <v>264</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B10" t="s">
+        <v>401</v>
+      </c>
+      <c r="C10" t="s">
+        <v>405</v>
+      </c>
+      <c r="D10" t="s">
+        <v>406</v>
+      </c>
+      <c r="E10" t="s">
+        <v>407</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B11" t="s">
+        <v>401</v>
+      </c>
+      <c r="C11" t="s">
+        <v>409</v>
+      </c>
+      <c r="D11" t="s">
+        <v>410</v>
+      </c>
+      <c r="E11" t="s">
+        <v>264</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B12" t="s">
+        <v>401</v>
+      </c>
+      <c r="C12" t="s">
+        <v>412</v>
+      </c>
+      <c r="D12" t="s">
+        <v>413</v>
+      </c>
+      <c r="E12" t="s">
+        <v>414</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B13" t="s">
+        <v>416</v>
+      </c>
+      <c r="C13" t="s">
+        <v>417</v>
+      </c>
+      <c r="D13" t="s">
+        <v>418</v>
+      </c>
+      <c r="E13" t="s">
+        <v>362</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B14" t="s">
+        <v>416</v>
+      </c>
+      <c r="C14" t="s">
+        <v>420</v>
+      </c>
+      <c r="D14" t="s">
+        <v>421</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B15" t="s">
+        <v>416</v>
+      </c>
+      <c r="C15" t="s">
+        <v>423</v>
+      </c>
+      <c r="D15" t="s">
+        <v>424</v>
+      </c>
+      <c r="E15" t="s">
+        <v>425</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B16" t="s">
+        <v>416</v>
+      </c>
+      <c r="C16" t="s">
+        <v>427</v>
+      </c>
+      <c r="D16" t="s">
+        <v>428</v>
+      </c>
+      <c r="E16" t="s">
+        <v>429</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B17" t="s">
+        <v>416</v>
+      </c>
+      <c r="C17" t="s">
+        <v>431</v>
+      </c>
+      <c r="D17" t="s">
+        <v>432</v>
+      </c>
+      <c r="E17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B18" t="s">
+        <v>416</v>
+      </c>
+      <c r="C18" t="s">
+        <v>434</v>
+      </c>
+      <c r="D18" t="s">
+        <v>435</v>
+      </c>
+      <c r="E18" t="s">
+        <v>436</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B19" t="s">
+        <v>416</v>
+      </c>
+      <c r="C19" t="s">
+        <v>438</v>
+      </c>
+      <c r="D19" t="s">
+        <v>439</v>
+      </c>
+      <c r="E19" t="s">
+        <v>244</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B20" t="s">
+        <v>416</v>
+      </c>
+      <c r="C20" t="s">
+        <v>441</v>
+      </c>
+      <c r="D20" t="s">
+        <v>442</v>
+      </c>
+      <c r="E20" t="s">
+        <v>436</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B21" t="s">
+        <v>416</v>
+      </c>
+      <c r="C21" t="s">
+        <v>444</v>
+      </c>
+      <c r="D21" t="s">
+        <v>445</v>
+      </c>
+      <c r="E21" t="s">
+        <v>446</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B22" t="s">
+        <v>416</v>
+      </c>
+      <c r="C22" t="s">
+        <v>448</v>
+      </c>
+      <c r="D22" t="s">
+        <v>449</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B23" t="s">
+        <v>416</v>
+      </c>
+      <c r="C23" t="s">
+        <v>451</v>
+      </c>
+      <c r="D23" t="s">
+        <v>452</v>
+      </c>
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B24" t="s">
+        <v>416</v>
+      </c>
+      <c r="C24" t="s">
+        <v>454</v>
+      </c>
+      <c r="D24" t="s">
+        <v>455</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B25" t="s">
+        <v>416</v>
+      </c>
+      <c r="C25" t="s">
+        <v>457</v>
+      </c>
+      <c r="D25" t="s">
+        <v>458</v>
+      </c>
+      <c r="E25" t="s">
+        <v>459</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B26" t="s">
+        <v>416</v>
+      </c>
+      <c r="C26" t="s">
+        <v>461</v>
+      </c>
+      <c r="D26" t="s">
+        <v>462</v>
+      </c>
+      <c r="E26" t="s">
+        <v>463</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B27" t="s">
+        <v>416</v>
+      </c>
+      <c r="C27" t="s">
+        <v>465</v>
+      </c>
+      <c r="D27" t="s">
+        <v>410</v>
+      </c>
+      <c r="E27" t="s">
+        <v>264</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B28" t="s">
+        <v>416</v>
+      </c>
+      <c r="C28" t="s">
+        <v>467</v>
+      </c>
+      <c r="D28" t="s">
+        <v>468</v>
+      </c>
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B29" t="s">
+        <v>416</v>
+      </c>
+      <c r="C29" t="s">
+        <v>470</v>
+      </c>
+      <c r="D29" t="s">
+        <v>471</v>
+      </c>
+      <c r="E29" t="s">
+        <v>407</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B30" t="s">
+        <v>416</v>
+      </c>
+      <c r="C30" t="s">
+        <v>473</v>
+      </c>
+      <c r="D30" t="s">
+        <v>474</v>
+      </c>
+      <c r="E30" t="s">
+        <v>264</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B31" t="s">
+        <v>416</v>
+      </c>
+      <c r="C31" t="s">
+        <v>476</v>
+      </c>
+      <c r="D31" t="s">
+        <v>477</v>
+      </c>
+      <c r="E31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B32" t="s">
+        <v>416</v>
+      </c>
+      <c r="C32" t="s">
+        <v>479</v>
+      </c>
+      <c r="D32" t="s">
+        <v>480</v>
+      </c>
+      <c r="E32" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B33" t="s">
+        <v>416</v>
+      </c>
+      <c r="C33" t="s">
+        <v>482</v>
+      </c>
+      <c r="D33" t="s">
+        <v>483</v>
+      </c>
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B34" t="s">
+        <v>416</v>
+      </c>
+      <c r="C34" t="s">
+        <v>485</v>
+      </c>
+      <c r="D34" t="s">
+        <v>486</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B35" t="s">
+        <v>416</v>
+      </c>
+      <c r="C35" t="s">
+        <v>488</v>
+      </c>
+      <c r="D35" t="s">
+        <v>489</v>
+      </c>
+      <c r="E35" t="s">
+        <v>490</v>
+      </c>
+      <c r="F35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B36" t="s">
+        <v>416</v>
+      </c>
+      <c r="C36" t="s">
+        <v>492</v>
+      </c>
+      <c r="D36" t="s">
+        <v>493</v>
+      </c>
+      <c r="E36" t="s">
+        <v>494</v>
+      </c>
+      <c r="F36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B37" t="s">
+        <v>416</v>
+      </c>
+      <c r="C37" t="s">
+        <v>496</v>
+      </c>
+      <c r="D37" t="s">
+        <v>497</v>
+      </c>
+      <c r="E37" t="s">
+        <v>498</v>
+      </c>
+      <c r="F37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B38" t="s">
+        <v>416</v>
+      </c>
+      <c r="C38" t="s">
+        <v>500</v>
+      </c>
+      <c r="D38" t="s">
+        <v>501</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B39" t="s">
+        <v>416</v>
+      </c>
+      <c r="C39" t="s">
+        <v>503</v>
+      </c>
+      <c r="D39" t="s">
+        <v>504</v>
+      </c>
+      <c r="E39" t="s">
+        <v>505</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B40" t="s">
+        <v>416</v>
+      </c>
+      <c r="C40" t="s">
+        <v>507</v>
+      </c>
+      <c r="D40" t="s">
+        <v>508</v>
+      </c>
+      <c r="E40" t="s">
+        <v>509</v>
+      </c>
+      <c r="F40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B41" t="s">
+        <v>416</v>
+      </c>
+      <c r="C41" t="s">
+        <v>511</v>
+      </c>
+      <c r="D41" t="s">
+        <v>512</v>
+      </c>
+      <c r="E41" t="s">
+        <v>268</v>
+      </c>
+      <c r="F41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B42" t="s">
+        <v>416</v>
+      </c>
+      <c r="C42" t="s">
+        <v>514</v>
+      </c>
+      <c r="D42" t="s">
+        <v>515</v>
+      </c>
+      <c r="E42" t="s">
+        <v>264</v>
+      </c>
+      <c r="F42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B43" t="s">
+        <v>416</v>
+      </c>
+      <c r="C43" t="s">
+        <v>517</v>
+      </c>
+      <c r="D43" t="s">
+        <v>518</v>
+      </c>
+      <c r="E43" t="s">
+        <v>264</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B44" t="s">
+        <v>416</v>
+      </c>
+      <c r="C44" t="s">
+        <v>520</v>
+      </c>
+      <c r="D44" t="s">
+        <v>521</v>
+      </c>
+      <c r="E44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B45" t="s">
+        <v>416</v>
+      </c>
+      <c r="C45" t="s">
+        <v>523</v>
+      </c>
+      <c r="D45" t="s">
+        <v>524</v>
+      </c>
+      <c r="E45" t="s">
+        <v>108</v>
+      </c>
+      <c r="F45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B46" t="s">
+        <v>416</v>
+      </c>
+      <c r="C46" t="s">
+        <v>526</v>
+      </c>
+      <c r="D46" t="s">
+        <v>527</v>
+      </c>
+      <c r="E46" t="s">
+        <v>264</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B47" t="s">
+        <v>416</v>
+      </c>
+      <c r="C47" t="s">
+        <v>529</v>
+      </c>
+      <c r="D47" t="s">
+        <v>530</v>
+      </c>
+      <c r="E47" t="s">
+        <v>531</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B48" t="s">
+        <v>416</v>
+      </c>
+      <c r="C48" t="s">
+        <v>533</v>
+      </c>
+      <c r="D48" t="s">
+        <v>534</v>
+      </c>
+      <c r="E48" t="s">
+        <v>264</v>
+      </c>
+      <c r="F48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B49" t="s">
+        <v>536</v>
+      </c>
+      <c r="C49" t="s">
+        <v>537</v>
+      </c>
+      <c r="D49" t="s">
+        <v>538</v>
+      </c>
+      <c r="E49" t="s">
+        <v>539</v>
+      </c>
+      <c r="F49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B50" t="s">
+        <v>536</v>
+      </c>
+      <c r="C50" t="s">
+        <v>541</v>
+      </c>
+      <c r="D50" t="s">
+        <v>542</v>
+      </c>
+      <c r="E50" t="s">
+        <v>543</v>
+      </c>
+      <c r="F50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B51" t="s">
+        <v>536</v>
+      </c>
+      <c r="C51" t="s">
+        <v>545</v>
+      </c>
+      <c r="D51" t="s">
+        <v>546</v>
+      </c>
+      <c r="E51" t="s">
+        <v>547</v>
+      </c>
+      <c r="F51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B52" t="s">
+        <v>549</v>
+      </c>
+      <c r="C52" t="s">
+        <v>550</v>
+      </c>
+      <c r="D52" t="s">
+        <v>551</v>
+      </c>
+      <c r="E52" t="s">
+        <v>39</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B53" t="s">
+        <v>549</v>
+      </c>
+      <c r="C53" t="s">
+        <v>553</v>
+      </c>
+      <c r="D53" t="s">
+        <v>554</v>
+      </c>
+      <c r="E53" t="s">
+        <v>39</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B54" t="s">
+        <v>549</v>
+      </c>
+      <c r="C54" t="s">
+        <v>556</v>
+      </c>
+      <c r="D54" t="s">
+        <v>557</v>
+      </c>
+      <c r="E54" t="s">
+        <v>39</v>
+      </c>
+      <c r="F54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B55" t="s">
+        <v>549</v>
+      </c>
+      <c r="C55" t="s">
+        <v>559</v>
+      </c>
+      <c r="D55" t="s">
+        <v>560</v>
+      </c>
+      <c r="E55" t="s">
+        <v>39</v>
+      </c>
+      <c r="F55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B56" t="s">
+        <v>549</v>
+      </c>
+      <c r="C56" t="s">
+        <v>562</v>
+      </c>
+      <c r="D56" t="s">
+        <v>563</v>
+      </c>
+      <c r="E56" t="s">
+        <v>39</v>
+      </c>
+      <c r="F56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B57" t="s">
+        <v>549</v>
+      </c>
+      <c r="C57" t="s">
+        <v>565</v>
+      </c>
+      <c r="D57" t="s">
+        <v>566</v>
+      </c>
+      <c r="E57" t="s">
+        <v>39</v>
+      </c>
+      <c r="F57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B58" t="s">
+        <v>549</v>
+      </c>
+      <c r="C58" t="s">
+        <v>568</v>
+      </c>
+      <c r="D58" t="s">
+        <v>569</v>
+      </c>
+      <c r="E58" t="s">
+        <v>39</v>
+      </c>
+      <c r="F58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B59" t="s">
+        <v>571</v>
+      </c>
+      <c r="C59" t="s">
+        <v>572</v>
+      </c>
+      <c r="D59" t="s">
+        <v>573</v>
+      </c>
+      <c r="E59" t="s">
+        <v>571</v>
+      </c>
+      <c r="F59" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B60" t="s">
+        <v>571</v>
+      </c>
+      <c r="C60" t="s">
+        <v>575</v>
+      </c>
+      <c r="D60" t="s">
+        <v>576</v>
+      </c>
+      <c r="E60" t="s">
+        <v>399</v>
+      </c>
+      <c r="F60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B61" t="s">
+        <v>571</v>
+      </c>
+      <c r="C61" t="s">
+        <v>578</v>
+      </c>
+      <c r="D61" t="s">
+        <v>579</v>
+      </c>
+      <c r="E61" t="s">
+        <v>571</v>
+      </c>
+      <c r="F61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B62" t="s">
+        <v>571</v>
+      </c>
+      <c r="C62" t="s">
+        <v>581</v>
+      </c>
+      <c r="D62" t="s">
+        <v>582</v>
+      </c>
+      <c r="E62" t="s">
+        <v>571</v>
+      </c>
+      <c r="F62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B63" t="s">
+        <v>571</v>
+      </c>
+      <c r="C63" t="s">
+        <v>584</v>
+      </c>
+      <c r="D63" t="s">
+        <v>585</v>
+      </c>
+      <c r="E63" t="s">
+        <v>571</v>
+      </c>
+      <c r="F63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B64" t="s">
+        <v>571</v>
+      </c>
+      <c r="C64" t="s">
+        <v>587</v>
+      </c>
+      <c r="D64" t="s">
+        <v>588</v>
+      </c>
+      <c r="E64" t="s">
+        <v>399</v>
+      </c>
+      <c r="F64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B65" t="s">
+        <v>571</v>
+      </c>
+      <c r="C65" t="s">
+        <v>590</v>
+      </c>
+      <c r="D65" t="s">
+        <v>591</v>
+      </c>
+      <c r="E65" t="s">
+        <v>399</v>
+      </c>
+      <c r="F65" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B66" t="s">
+        <v>571</v>
+      </c>
+      <c r="C66" t="s">
+        <v>593</v>
+      </c>
+      <c r="D66" t="s">
+        <v>594</v>
+      </c>
+      <c r="E66" t="s">
+        <v>399</v>
+      </c>
+      <c r="F66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B67" t="s">
+        <v>571</v>
+      </c>
+      <c r="C67" t="s">
+        <v>596</v>
+      </c>
+      <c r="D67" t="s">
+        <v>597</v>
+      </c>
+      <c r="E67" t="s">
+        <v>399</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
quality index rules complete
</commit_message>
<xml_diff>
--- a/files/Rule-Sets.xlsx
+++ b/files/Rule-Sets.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="120" windowWidth="20868" windowHeight="7416" activeTab="1"/>
+    <workbookView xWindow="672" yWindow="120" windowWidth="20868" windowHeight="7416" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Elements of Java Style" sheetId="1" r:id="rId1"/>
     <sheet name="Clean Code" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Code Quality Index" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Ruleset_Clean_Code" localSheetId="1">'Clean Code'!$A$1:$F$67</definedName>
+    <definedName name="Ruleset_Code_Quality_Index" localSheetId="2">'Code Quality Index'!$A$1:$F$53</definedName>
     <definedName name="Ruleset_Elements_Of_Java_Style" localSheetId="0">'Elements of Java Style'!$A$1:$F$109</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -33,7 +34,19 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="Ruleset_Elements-Of-Java-Style" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="2" name="Ruleset_Code-Quality-Index" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\Develop\Diplom\git_repo\files\Ruleset_Code-Quality-Index.csv" decimal="," thousands="." tab="0" semicolon="1" qualifier="none">
+      <textFields count="6">
+        <textField type="text"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="Ruleset_Elements-Of-Java-Style" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\jnru\Desktop\Ruleset_Elements-Of-Java-Style.csv" decimal="," thousands="." tab="0" semicolon="1" qualifier="none">
       <textFields count="6">
         <textField type="text"/>
@@ -49,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="770">
   <si>
     <t>ID</t>
   </si>
@@ -1843,6 +1856,522 @@
   </si>
   <si>
     <t>Tests bestmöglich beschleunigen</t>
+  </si>
+  <si>
+    <t>CQI-001</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Allgemeine Parameter</t>
+  </si>
+  <si>
+    <t>Casting von Methodenparametern vermeiden (außer bei Überschriebenen Methoden)</t>
+  </si>
+  <si>
+    <t>CQI-002</t>
+  </si>
+  <si>
+    <t>Attributüberdeckung</t>
+  </si>
+  <si>
+    <t>Verwenden gleicher Variablennamen in Unterklassen vermeiden</t>
+  </si>
+  <si>
+    <t>Variables, Inheritance</t>
+  </si>
+  <si>
+    <t>CQI-003</t>
+  </si>
+  <si>
+    <t>Ausgeschlagenes Erbe - Implementierung</t>
+  </si>
+  <si>
+    <t>Methodenimplementierung von Oberklasse sollte von Mehrheit der Unterklassen nicht überschrieben werden</t>
+  </si>
+  <si>
+    <t>Methods, Inheritance</t>
+  </si>
+  <si>
+    <t>CQI-004</t>
+  </si>
+  <si>
+    <t>Ausgeschlagenes Erbe - Schnittstelle</t>
+  </si>
+  <si>
+    <t>Reduktion von Sichtbarkeiten in Unterklassen und Leer-Implementierung von Schnittstellen vermeiden</t>
+  </si>
+  <si>
+    <t>CQi-005</t>
+  </si>
+  <si>
+    <t>Datenkapselaufbruch</t>
+  </si>
+  <si>
+    <t>Keine public Klassenvariablen verwenden (außer Konstanten)</t>
+  </si>
+  <si>
+    <t>CQI-006</t>
+  </si>
+  <si>
+    <t>Technologie</t>
+  </si>
+  <si>
+    <t>Duplizierter Code</t>
+  </si>
+  <si>
+    <t>Duplizierten Code vermeiden (&gt;40 aufeinander folgende Zeilen)</t>
+  </si>
+  <si>
+    <t>CQI-007</t>
+  </si>
+  <si>
+    <t>Falsche Namenslänge</t>
+  </si>
+  <si>
+    <t>Namen &lt;2 oder &gt;50 Zeichen nicht verwenden</t>
+  </si>
+  <si>
+    <t>CQI-008</t>
+  </si>
+  <si>
+    <t>Generationskonflikt</t>
+  </si>
+  <si>
+    <t>Erbende Klassen sollten weniger als die Hälfte der Oberklasse überschreiben ohne die Oberklassenimplementierung zu benutzen</t>
+  </si>
+  <si>
+    <t>CQI-009</t>
+  </si>
+  <si>
+    <t>Gottdatei</t>
+  </si>
+  <si>
+    <t>Dateien sollten weniger als 2000 Zeilen enthalten</t>
+  </si>
+  <si>
+    <t>CQI-010</t>
+  </si>
+  <si>
+    <t>Gottklasse (Attribut)</t>
+  </si>
+  <si>
+    <t>Klassen sollten weniger als 50 Klassenvariablen deklarieren (außer Konstanten)</t>
+  </si>
+  <si>
+    <t>Classes, Variables</t>
+  </si>
+  <si>
+    <t>CQI-011</t>
+  </si>
+  <si>
+    <t>Gottklasse (Methode)</t>
+  </si>
+  <si>
+    <t>Eine Klasse sollte weniger als 50 Methoden deklarieren</t>
+  </si>
+  <si>
+    <t>CQI-012</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Gottmethode</t>
+  </si>
+  <si>
+    <t>Eine Methode sollte weniger als 200 Zeilen haben</t>
+  </si>
+  <si>
+    <t>CQI-013</t>
+  </si>
+  <si>
+    <t>Architektur</t>
+  </si>
+  <si>
+    <t>Gottpaket</t>
+  </si>
+  <si>
+    <t>In einem package sollten höchstens 50 Klassen und Interfaces deklariert werden</t>
+  </si>
+  <si>
+    <t>Classes, Structure</t>
+  </si>
+  <si>
+    <t>CQI-014</t>
+  </si>
+  <si>
+    <t>Halbherzige Operationen</t>
+  </si>
+  <si>
+    <t>Klassen die equals() implementieren sollten auch die hashCode() implementieren</t>
+  </si>
+  <si>
+    <t>CQI-015</t>
+  </si>
+  <si>
+    <t>Heimliche Verwandschaft</t>
+  </si>
+  <si>
+    <t>public Methoden einer Oberklasse sollten nicht nur von erbenden Klassen verwendet werden</t>
+  </si>
+  <si>
+    <t>CQI-016</t>
+  </si>
+  <si>
+    <t>Identitätsspaltung</t>
+  </si>
+  <si>
+    <t>Klassen in einem System sollten nicht den gleichen Namen haben oder sich nur durch groß/kleinschreibung unterscheiden</t>
+  </si>
+  <si>
+    <t>CQI-017</t>
+  </si>
+  <si>
+    <t>Importchaos</t>
+  </si>
+  <si>
+    <t>Imports nicht doppelt, aus gleichem package, von java.lang oder als wildcard</t>
+  </si>
+  <si>
+    <t>CQI-018</t>
+  </si>
+  <si>
+    <t>Importlüge</t>
+  </si>
+  <si>
+    <t>Unbenutzte Imports entfernen</t>
+  </si>
+  <si>
+    <t>Import, Unused</t>
+  </si>
+  <si>
+    <t>CQI-019</t>
+  </si>
+  <si>
+    <t>Informelle Dokumentation</t>
+  </si>
+  <si>
+    <t>Public Methoden müssen formal kommentiert werden (mit /*, z.B JavaDoc)</t>
+  </si>
+  <si>
+    <t>CQI-020</t>
+  </si>
+  <si>
+    <t>Interface-Bypass</t>
+  </si>
+  <si>
+    <t>Implementation eines Methodeninterfaces sollten nicht direkt genutzt werden sondern über abstraktes Interface</t>
+  </si>
+  <si>
+    <t>Inheritance, Methods</t>
+  </si>
+  <si>
+    <t>CQI-021</t>
+  </si>
+  <si>
+    <t>Klässchen</t>
+  </si>
+  <si>
+    <t>Öffentlich sichtbare Klassen sollten mindestens 3 Methoden oder 3 Klassenvariablen haben</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>CQI-022</t>
+  </si>
+  <si>
+    <t>klasseninzest</t>
+  </si>
+  <si>
+    <t>Oberklassen dürfen keine Referenzen auf erbende Klassen enthalten</t>
+  </si>
+  <si>
+    <t>CQI-023</t>
+  </si>
+  <si>
+    <t>Konstantenregen</t>
+  </si>
+  <si>
+    <t>Namen von Konstanten sollten nur einmal im System vorkommen</t>
+  </si>
+  <si>
+    <t>CQI-024</t>
+  </si>
+  <si>
+    <t>Labyrinthmethode</t>
+  </si>
+  <si>
+    <t>Die McCabe-Komplexität einer Methode sollte nicht &gt;10 sein</t>
+  </si>
+  <si>
+    <t>Conditionals, Methods</t>
+  </si>
+  <si>
+    <t>CQI-025</t>
+  </si>
+  <si>
+    <t>Lange Parameterliste</t>
+  </si>
+  <si>
+    <t>Methoden sollten nicht mehr als 7 Parameter haben</t>
+  </si>
+  <si>
+    <t>CQI-026</t>
+  </si>
+  <si>
+    <t>Maskierende Datei</t>
+  </si>
+  <si>
+    <t>Der Dateiname sollte in enthaltener Klasse vollständig vorkommen</t>
+  </si>
+  <si>
+    <t>CQI-027</t>
+  </si>
+  <si>
+    <t>Nachlässige Kommentierung</t>
+  </si>
+  <si>
+    <t>Je Codezeile möglichst eine Kommentarzeile - (Dateizeilen - 2*Kommentarzeilen) möglichst klein</t>
+  </si>
+  <si>
+    <t>CQI-028</t>
+  </si>
+  <si>
+    <t>Namensfehler</t>
+  </si>
+  <si>
+    <t>Standard-Java-Namenskonventionen sollten eingehalten werden</t>
+  </si>
+  <si>
+    <t>CQI-029</t>
+  </si>
+  <si>
+    <t>Objektplacebo (Attribut)</t>
+  </si>
+  <si>
+    <t>Statische Attribute sollten nur über Objekttyp statisch referenziert werden</t>
+  </si>
+  <si>
+    <t>CQI-030</t>
+  </si>
+  <si>
+    <t>Objectplacebo (Methode)</t>
+  </si>
+  <si>
+    <t>Statische Methoden sollten nur über Objekttyp statisch referenziert werden</t>
+  </si>
+  <si>
+    <t>CQI-031</t>
+  </si>
+  <si>
+    <t>Paketchen</t>
+  </si>
+  <si>
+    <t>Nichtleere Pakete sollten mindestens 3 öffentliche Klassen / Interfaces enthalten</t>
+  </si>
+  <si>
+    <t>CQI-032</t>
+  </si>
+  <si>
+    <t>Pakethierarchieaufbruch</t>
+  </si>
+  <si>
+    <t>Oberklassen sollten nicht in untergeordneten Paketen liegen, wenn erbende Klassen in übergeordneten Paketen liegen</t>
+  </si>
+  <si>
+    <t>CQI-033</t>
+  </si>
+  <si>
+    <t>Polymorphieplacebo</t>
+  </si>
+  <si>
+    <t>Statische Methoden der Oberklasse sollten nicht in erbenden Klassen überdeckt werden</t>
+  </si>
+  <si>
+    <t>CQI-034</t>
+  </si>
+  <si>
+    <t>Potenzielle Privatsphäre (Attribut)</t>
+  </si>
+  <si>
+    <t>Sichtbarkeiten von Variablen sollten so weit wie möglich eingeschränkt werden</t>
+  </si>
+  <si>
+    <t>CQI-035</t>
+  </si>
+  <si>
+    <t>Potenzielle Privatsphäre (Methode)</t>
+  </si>
+  <si>
+    <t>Methoden sollten nur protected deklariert werden wenn sie eine Methode der Oberklasse überschreiben oder von Unterklassen überschrieben werden</t>
+  </si>
+  <si>
+    <t>CQI-036</t>
+  </si>
+  <si>
+    <t>Pränatale Kommunikation</t>
+  </si>
+  <si>
+    <t>In Konstruktoren sollten keine virtuellen Methoden aufgerufen werden</t>
+  </si>
+  <si>
+    <t>CQI-037</t>
+  </si>
+  <si>
+    <t>Risikocode</t>
+  </si>
+  <si>
+    <t>Case-Anweisungen sollten mit break abgeschlossen werden, switch-Anweisungen sollten einen default-case enthalten und Catch-Anweisungen sollten nicht leer sein</t>
+  </si>
+  <si>
+    <t>Exceptions, Conditionals</t>
+  </si>
+  <si>
+    <t>CQI-038</t>
+  </si>
+  <si>
+    <t>Signaturähnliche Klassen</t>
+  </si>
+  <si>
+    <t>Nicht durch Vererbung zusammenhängende Klassen sollten weniger als 50% identische Methodensignaturen enthalten</t>
+  </si>
+  <si>
+    <t>CQI-039</t>
+  </si>
+  <si>
+    <t>Simulierte Polymorphie</t>
+  </si>
+  <si>
+    <t>Objekte sollten in einer Methode nicht auf mehrere Objekttypen überprüft werden (durch instanceof)</t>
+  </si>
+  <si>
+    <t>CQI-040</t>
+  </si>
+  <si>
+    <t>Späte Abstraktion</t>
+  </si>
+  <si>
+    <t>Abstrakte Klassen sollten nicht von nicht-abstrakten Klassen erben</t>
+  </si>
+  <si>
+    <t>CQI-041</t>
+  </si>
+  <si>
+    <t>Tote Attribute</t>
+  </si>
+  <si>
+    <t>Ungenutzte private Variablen sollten entfernt werden</t>
+  </si>
+  <si>
+    <t>Unused, Variables</t>
+  </si>
+  <si>
+    <t>CQI-042</t>
+  </si>
+  <si>
+    <t>Tote Implementierung</t>
+  </si>
+  <si>
+    <t>Anweisungen die nie ausgeführt werden sollten netfernt werden</t>
+  </si>
+  <si>
+    <t>CQI-043</t>
+  </si>
+  <si>
+    <t>Tote Methoden</t>
+  </si>
+  <si>
+    <t>Ungenutzte private Methoden sollten entfernt werden</t>
+  </si>
+  <si>
+    <t>CQI-044</t>
+  </si>
+  <si>
+    <t>Überbuchte Datei</t>
+  </si>
+  <si>
+    <t>Eine Datei sollte nur eine übergeordnete public Klasse enthalten</t>
+  </si>
+  <si>
+    <t>CQI-045</t>
+  </si>
+  <si>
+    <t>Unfertiger Code</t>
+  </si>
+  <si>
+    <t>ToDo / FixMe / Hack - Kommentare sollten behoben werden</t>
+  </si>
+  <si>
+    <t>CQI-046</t>
+  </si>
+  <si>
+    <t>Unvollständige Vererbung (Attribut)</t>
+  </si>
+  <si>
+    <t>Eine nicht-statische Variable sollte nicht in mehr als 50% (+ mehr als 2) der erbenden Klassen einer Oberklasse namensgleich vorkommen</t>
+  </si>
+  <si>
+    <t>Inheritance, Variables</t>
+  </si>
+  <si>
+    <t>CQI-047</t>
+  </si>
+  <si>
+    <t>Unvollständige Vererbung (Methode)</t>
+  </si>
+  <si>
+    <t>Eine Methodensignatur sollte nicht in mehr als 50% (+ mehr als 2) der erbenden Klassen einer Oberklasse namensgleich vorkommen</t>
+  </si>
+  <si>
+    <t>CQI-048</t>
+  </si>
+  <si>
+    <t>Verbotene Dateiliebe</t>
+  </si>
+  <si>
+    <t>Zwei Dateien sollten nicht gegenseitig voneinander Abhängen</t>
+  </si>
+  <si>
+    <t>Structure, Import</t>
+  </si>
+  <si>
+    <t>CQI-049</t>
+  </si>
+  <si>
+    <t>Verbotene Klassenliebe</t>
+  </si>
+  <si>
+    <t>Zwei nicht durch Vererbung zusammenhängende Klassen sollten nicht gegenseitig voneinander abhängen</t>
+  </si>
+  <si>
+    <t>CQI-050</t>
+  </si>
+  <si>
+    <t>Verbotene Methodenliebe</t>
+  </si>
+  <si>
+    <t>Zwei Methoden sollten sich nicht gegenseitig aufrufen</t>
+  </si>
+  <si>
+    <t>CQI-051</t>
+  </si>
+  <si>
+    <t>Verbotene Paketliebe</t>
+  </si>
+  <si>
+    <t>Zwei Pakete sollten sich nicht gegenseitig zum kompilieren benötigen</t>
+  </si>
+  <si>
+    <t>CQI-052</t>
+  </si>
+  <si>
+    <t>Versteckte Konstantheit</t>
+  </si>
+  <si>
+    <t>Klassenvariablen die nach initialisierung nicht verändert werden sollten als final deklariert werden</t>
   </si>
 </sst>
 </file>
@@ -1896,11 +2425,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Ruleset_Elements-Of-Java-Style" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Ruleset_Elements-Of-Java-Style" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Ruleset_Clean-Code" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Ruleset_Code-Quality-Index" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4395,7 +4928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5750,12 +6283,1081 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C2" t="s">
+        <v>600</v>
+      </c>
+      <c r="D2" t="s">
+        <v>601</v>
+      </c>
+      <c r="E2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B3" t="s">
+        <v>599</v>
+      </c>
+      <c r="C3" t="s">
+        <v>603</v>
+      </c>
+      <c r="D3" t="s">
+        <v>604</v>
+      </c>
+      <c r="E3" t="s">
+        <v>605</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C4" t="s">
+        <v>607</v>
+      </c>
+      <c r="D4" t="s">
+        <v>608</v>
+      </c>
+      <c r="E4" t="s">
+        <v>609</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="B5" t="s">
+        <v>599</v>
+      </c>
+      <c r="C5" t="s">
+        <v>611</v>
+      </c>
+      <c r="D5" t="s">
+        <v>612</v>
+      </c>
+      <c r="E5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B6" t="s">
+        <v>599</v>
+      </c>
+      <c r="C6" t="s">
+        <v>614</v>
+      </c>
+      <c r="D6" t="s">
+        <v>615</v>
+      </c>
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C7" t="s">
+        <v>618</v>
+      </c>
+      <c r="D7" t="s">
+        <v>619</v>
+      </c>
+      <c r="E7" t="s">
+        <v>264</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B8" t="s">
+        <v>617</v>
+      </c>
+      <c r="C8" t="s">
+        <v>621</v>
+      </c>
+      <c r="D8" t="s">
+        <v>622</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="B9" t="s">
+        <v>599</v>
+      </c>
+      <c r="C9" t="s">
+        <v>624</v>
+      </c>
+      <c r="D9" t="s">
+        <v>625</v>
+      </c>
+      <c r="E9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B10" t="s">
+        <v>599</v>
+      </c>
+      <c r="C10" t="s">
+        <v>627</v>
+      </c>
+      <c r="D10" t="s">
+        <v>628</v>
+      </c>
+      <c r="E10" t="s">
+        <v>362</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B11" t="s">
+        <v>599</v>
+      </c>
+      <c r="C11" t="s">
+        <v>630</v>
+      </c>
+      <c r="D11" t="s">
+        <v>631</v>
+      </c>
+      <c r="E11" t="s">
+        <v>632</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B12" t="s">
+        <v>599</v>
+      </c>
+      <c r="C12" t="s">
+        <v>634</v>
+      </c>
+      <c r="D12" t="s">
+        <v>635</v>
+      </c>
+      <c r="E12" t="s">
+        <v>436</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B13" t="s">
+        <v>637</v>
+      </c>
+      <c r="C13" t="s">
+        <v>638</v>
+      </c>
+      <c r="D13" t="s">
+        <v>639</v>
+      </c>
+      <c r="E13" t="s">
+        <v>264</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B14" t="s">
+        <v>641</v>
+      </c>
+      <c r="C14" t="s">
+        <v>642</v>
+      </c>
+      <c r="D14" t="s">
+        <v>643</v>
+      </c>
+      <c r="E14" t="s">
+        <v>644</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B15" t="s">
+        <v>599</v>
+      </c>
+      <c r="C15" t="s">
+        <v>646</v>
+      </c>
+      <c r="D15" t="s">
+        <v>647</v>
+      </c>
+      <c r="E15" t="s">
+        <v>609</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B16" t="s">
+        <v>599</v>
+      </c>
+      <c r="C16" t="s">
+        <v>649</v>
+      </c>
+      <c r="D16" t="s">
+        <v>650</v>
+      </c>
+      <c r="E16" t="s">
+        <v>609</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B17" t="s">
+        <v>599</v>
+      </c>
+      <c r="C17" t="s">
+        <v>652</v>
+      </c>
+      <c r="D17" t="s">
+        <v>653</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B18" t="s">
+        <v>637</v>
+      </c>
+      <c r="C18" t="s">
+        <v>655</v>
+      </c>
+      <c r="D18" t="s">
+        <v>656</v>
+      </c>
+      <c r="E18" t="s">
+        <v>539</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B19" t="s">
+        <v>637</v>
+      </c>
+      <c r="C19" t="s">
+        <v>658</v>
+      </c>
+      <c r="D19" t="s">
+        <v>659</v>
+      </c>
+      <c r="E19" t="s">
+        <v>660</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="B20" t="s">
+        <v>637</v>
+      </c>
+      <c r="C20" t="s">
+        <v>662</v>
+      </c>
+      <c r="D20" t="s">
+        <v>663</v>
+      </c>
+      <c r="E20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="B21" t="s">
+        <v>599</v>
+      </c>
+      <c r="C21" t="s">
+        <v>665</v>
+      </c>
+      <c r="D21" t="s">
+        <v>666</v>
+      </c>
+      <c r="E21" t="s">
+        <v>667</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B22" t="s">
+        <v>599</v>
+      </c>
+      <c r="C22" t="s">
+        <v>669</v>
+      </c>
+      <c r="D22" t="s">
+        <v>670</v>
+      </c>
+      <c r="E22" t="s">
+        <v>671</v>
+      </c>
+      <c r="F22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B23" t="s">
+        <v>599</v>
+      </c>
+      <c r="C23" t="s">
+        <v>673</v>
+      </c>
+      <c r="D23" t="s">
+        <v>674</v>
+      </c>
+      <c r="E23" t="s">
+        <v>244</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="B24" t="s">
+        <v>617</v>
+      </c>
+      <c r="C24" t="s">
+        <v>676</v>
+      </c>
+      <c r="D24" t="s">
+        <v>677</v>
+      </c>
+      <c r="E24" t="s">
+        <v>498</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="B25" t="s">
+        <v>637</v>
+      </c>
+      <c r="C25" t="s">
+        <v>679</v>
+      </c>
+      <c r="D25" t="s">
+        <v>680</v>
+      </c>
+      <c r="E25" t="s">
+        <v>681</v>
+      </c>
+      <c r="F25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B26" t="s">
+        <v>599</v>
+      </c>
+      <c r="C26" t="s">
+        <v>683</v>
+      </c>
+      <c r="D26" t="s">
+        <v>684</v>
+      </c>
+      <c r="E26" t="s">
+        <v>264</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="B27" t="s">
+        <v>617</v>
+      </c>
+      <c r="C27" t="s">
+        <v>686</v>
+      </c>
+      <c r="D27" t="s">
+        <v>687</v>
+      </c>
+      <c r="E27" t="s">
+        <v>644</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="B28" t="s">
+        <v>617</v>
+      </c>
+      <c r="C28" t="s">
+        <v>689</v>
+      </c>
+      <c r="D28" t="s">
+        <v>690</v>
+      </c>
+      <c r="E28" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="B29" t="s">
+        <v>617</v>
+      </c>
+      <c r="C29" t="s">
+        <v>692</v>
+      </c>
+      <c r="D29" t="s">
+        <v>693</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B30" t="s">
+        <v>637</v>
+      </c>
+      <c r="C30" t="s">
+        <v>695</v>
+      </c>
+      <c r="D30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="B31" t="s">
+        <v>637</v>
+      </c>
+      <c r="C31" t="s">
+        <v>698</v>
+      </c>
+      <c r="D31" t="s">
+        <v>699</v>
+      </c>
+      <c r="E31" t="s">
+        <v>264</v>
+      </c>
+      <c r="F31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B32" t="s">
+        <v>641</v>
+      </c>
+      <c r="C32" t="s">
+        <v>701</v>
+      </c>
+      <c r="D32" t="s">
+        <v>702</v>
+      </c>
+      <c r="E32" t="s">
+        <v>644</v>
+      </c>
+      <c r="F32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B33" t="s">
+        <v>641</v>
+      </c>
+      <c r="C33" t="s">
+        <v>704</v>
+      </c>
+      <c r="D33" t="s">
+        <v>705</v>
+      </c>
+      <c r="E33" t="s">
+        <v>505</v>
+      </c>
+      <c r="F33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="B34" t="s">
+        <v>599</v>
+      </c>
+      <c r="C34" t="s">
+        <v>707</v>
+      </c>
+      <c r="D34" t="s">
+        <v>708</v>
+      </c>
+      <c r="E34" t="s">
+        <v>667</v>
+      </c>
+      <c r="F34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="B35" t="s">
+        <v>599</v>
+      </c>
+      <c r="C35" t="s">
+        <v>710</v>
+      </c>
+      <c r="D35" t="s">
+        <v>711</v>
+      </c>
+      <c r="E35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B36" t="s">
+        <v>599</v>
+      </c>
+      <c r="C36" t="s">
+        <v>713</v>
+      </c>
+      <c r="D36" t="s">
+        <v>714</v>
+      </c>
+      <c r="E36" t="s">
+        <v>609</v>
+      </c>
+      <c r="F36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B37" t="s">
+        <v>599</v>
+      </c>
+      <c r="C37" t="s">
+        <v>716</v>
+      </c>
+      <c r="D37" t="s">
+        <v>717</v>
+      </c>
+      <c r="E37" t="s">
+        <v>667</v>
+      </c>
+      <c r="F37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B38" t="s">
+        <v>637</v>
+      </c>
+      <c r="C38" t="s">
+        <v>719</v>
+      </c>
+      <c r="D38" t="s">
+        <v>720</v>
+      </c>
+      <c r="E38" t="s">
+        <v>721</v>
+      </c>
+      <c r="F38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B39" t="s">
+        <v>599</v>
+      </c>
+      <c r="C39" t="s">
+        <v>723</v>
+      </c>
+      <c r="D39" t="s">
+        <v>724</v>
+      </c>
+      <c r="E39" t="s">
+        <v>436</v>
+      </c>
+      <c r="F39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B40" t="s">
+        <v>637</v>
+      </c>
+      <c r="C40" t="s">
+        <v>726</v>
+      </c>
+      <c r="D40" t="s">
+        <v>727</v>
+      </c>
+      <c r="E40" t="s">
+        <v>244</v>
+      </c>
+      <c r="F40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B41" t="s">
+        <v>599</v>
+      </c>
+      <c r="C41" t="s">
+        <v>729</v>
+      </c>
+      <c r="D41" t="s">
+        <v>730</v>
+      </c>
+      <c r="E41" t="s">
+        <v>244</v>
+      </c>
+      <c r="F41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="B42" t="s">
+        <v>599</v>
+      </c>
+      <c r="C42" t="s">
+        <v>732</v>
+      </c>
+      <c r="D42" t="s">
+        <v>733</v>
+      </c>
+      <c r="E42" t="s">
+        <v>734</v>
+      </c>
+      <c r="F42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B43" t="s">
+        <v>637</v>
+      </c>
+      <c r="C43" t="s">
+        <v>736</v>
+      </c>
+      <c r="D43" t="s">
+        <v>737</v>
+      </c>
+      <c r="E43" t="s">
+        <v>446</v>
+      </c>
+      <c r="F43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="B44" t="s">
+        <v>599</v>
+      </c>
+      <c r="C44" t="s">
+        <v>739</v>
+      </c>
+      <c r="D44" t="s">
+        <v>740</v>
+      </c>
+      <c r="E44" t="s">
+        <v>414</v>
+      </c>
+      <c r="F44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B45" t="s">
+        <v>599</v>
+      </c>
+      <c r="C45" t="s">
+        <v>742</v>
+      </c>
+      <c r="D45" t="s">
+        <v>743</v>
+      </c>
+      <c r="E45" t="s">
+        <v>644</v>
+      </c>
+      <c r="F45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B46" t="s">
+        <v>637</v>
+      </c>
+      <c r="C46" t="s">
+        <v>745</v>
+      </c>
+      <c r="D46" t="s">
+        <v>746</v>
+      </c>
+      <c r="E46" t="s">
+        <v>120</v>
+      </c>
+      <c r="F46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B47" t="s">
+        <v>599</v>
+      </c>
+      <c r="C47" t="s">
+        <v>748</v>
+      </c>
+      <c r="D47" t="s">
+        <v>749</v>
+      </c>
+      <c r="E47" t="s">
+        <v>750</v>
+      </c>
+      <c r="F47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B48" t="s">
+        <v>599</v>
+      </c>
+      <c r="C48" t="s">
+        <v>752</v>
+      </c>
+      <c r="D48" t="s">
+        <v>753</v>
+      </c>
+      <c r="E48" t="s">
+        <v>667</v>
+      </c>
+      <c r="F48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B49" t="s">
+        <v>599</v>
+      </c>
+      <c r="C49" t="s">
+        <v>755</v>
+      </c>
+      <c r="D49" t="s">
+        <v>756</v>
+      </c>
+      <c r="E49" t="s">
+        <v>757</v>
+      </c>
+      <c r="F49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B50" t="s">
+        <v>599</v>
+      </c>
+      <c r="C50" t="s">
+        <v>759</v>
+      </c>
+      <c r="D50" t="s">
+        <v>760</v>
+      </c>
+      <c r="E50" t="s">
+        <v>671</v>
+      </c>
+      <c r="F50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B51" t="s">
+        <v>599</v>
+      </c>
+      <c r="C51" t="s">
+        <v>762</v>
+      </c>
+      <c r="D51" t="s">
+        <v>763</v>
+      </c>
+      <c r="E51" t="s">
+        <v>264</v>
+      </c>
+      <c r="F51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B52" t="s">
+        <v>641</v>
+      </c>
+      <c r="C52" t="s">
+        <v>765</v>
+      </c>
+      <c r="D52" t="s">
+        <v>766</v>
+      </c>
+      <c r="E52" t="s">
+        <v>362</v>
+      </c>
+      <c r="F52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B53" t="s">
+        <v>599</v>
+      </c>
+      <c r="C53" t="s">
+        <v>768</v>
+      </c>
+      <c r="D53" t="s">
+        <v>769</v>
+      </c>
+      <c r="E53" t="s">
+        <v>108</v>
+      </c>
+      <c r="F53" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Java Coding guidelines rules half
</commit_message>
<xml_diff>
--- a/files/Rule-Sets.xlsx
+++ b/files/Rule-Sets.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="120" windowWidth="20868" windowHeight="7416" activeTab="2"/>
+    <workbookView xWindow="672" yWindow="120" windowWidth="20868" windowHeight="7416" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Elements of Java Style" sheetId="1" r:id="rId1"/>
     <sheet name="Clean Code" sheetId="2" r:id="rId2"/>
     <sheet name="Code Quality Index" sheetId="3" r:id="rId3"/>
+    <sheet name="Java Coding Guidelines" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Ruleset_Clean_Code" localSheetId="1">'Clean Code'!$A$1:$F$67</definedName>
@@ -2725,7 +2726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D85" workbookViewId="0">
       <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
@@ -4928,7 +4929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A46" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6285,7 +6286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7360,4 +7361,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
sopra dortmund rules complete
</commit_message>
<xml_diff>
--- a/files/Rule-Sets.xlsx
+++ b/files/Rule-Sets.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="120" windowWidth="20868" windowHeight="7416" activeTab="3"/>
+    <workbookView xWindow="672" yWindow="120" windowWidth="20868" windowHeight="7416" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Elements of Java Style" sheetId="1" r:id="rId1"/>
     <sheet name="Clean Code" sheetId="2" r:id="rId2"/>
     <sheet name="Code Quality Index" sheetId="3" r:id="rId3"/>
     <sheet name="Java Coding Guidelines" sheetId="4" r:id="rId4"/>
+    <sheet name="SoPra Dortmund" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Ruleset_Clean_Code" localSheetId="1">'Clean Code'!$A$1:$F$67</definedName>
     <definedName name="Ruleset_Code_Quality_Index" localSheetId="2">'Code Quality Index'!$A$1:$F$53</definedName>
     <definedName name="Ruleset_Elements_Of_Java_Style" localSheetId="0">'Elements of Java Style'!$A$1:$F$109</definedName>
+    <definedName name="Ruleset_Java_Coding_Guidelines" localSheetId="3">'Java Coding Guidelines'!$A$1:$F$76</definedName>
+    <definedName name="Ruleset_Softwarepraktikum_Dortmund" localSheetId="4">'SoPra Dortmund'!$A$1:$F$12</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -59,11 +62,35 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="4" name="Ruleset_Java-Coding-Guidelines" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\Develop\Diplom\git_repo\files\Ruleset_Java-Coding-Guidelines.csv" decimal="," thousands="." tab="0" semicolon="1" qualifier="none">
+      <textFields count="6">
+        <textField type="text"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="Ruleset_Softwarepraktikum-Dortmund" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\Develop\Diplom\git_repo\files\Ruleset_Softwarepraktikum-Dortmund.csv" decimal="," thousands="." tab="0" semicolon="1" qualifier="none">
+      <textFields count="6">
+        <textField type="text"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="1055">
   <si>
     <t>ID</t>
   </si>
@@ -2373,6 +2400,861 @@
   </si>
   <si>
     <t>Klassenvariablen die nach initialisierung nicht verändert werden sollten als final deklariert werden</t>
+  </si>
+  <si>
+    <t>JCG-001</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Limit the lifetime of sensitive data</t>
+  </si>
+  <si>
+    <t>Sicherheitskritische Daten nur so kurz wie möglich im Speicher halten</t>
+  </si>
+  <si>
+    <t>JCG-002</t>
+  </si>
+  <si>
+    <t>Do not store unencrypted sensitive information on the client side</t>
+  </si>
+  <si>
+    <t>Keine kritischen Daten (Wie Passwörter) unverschlüsselt auf Client-Seite (Cookie) halten</t>
+  </si>
+  <si>
+    <t>JCG-003</t>
+  </si>
+  <si>
+    <t>Provide sensitive mutable classes with unmodifiable wrappers</t>
+  </si>
+  <si>
+    <t>Sicherheitskritische mutable Klassen sollten eingekapselt werden, sodass unerlaubte Schreiboperationen verhindert werden</t>
+  </si>
+  <si>
+    <t>JCG-004</t>
+  </si>
+  <si>
+    <t>Ensure that security-sensitive methods are called with validated arguments</t>
+  </si>
+  <si>
+    <t>Argumente die an sicherheitskritische Methoden gegeben werden sollten vorher validiert werden</t>
+  </si>
+  <si>
+    <t>Security, Methods</t>
+  </si>
+  <si>
+    <t>JCG-005</t>
+  </si>
+  <si>
+    <t>Prevent arbitrary file upload</t>
+  </si>
+  <si>
+    <t>Uploads von beliebigen Dateitypen sollte verhindert werden</t>
+  </si>
+  <si>
+    <t>Security, InOut</t>
+  </si>
+  <si>
+    <t>JCG-006</t>
+  </si>
+  <si>
+    <t>Properly encode or escape output</t>
+  </si>
+  <si>
+    <t>Jeglicher Output sollte zuvor überprüft und normalisiert werden</t>
+  </si>
+  <si>
+    <t>JCG-007</t>
+  </si>
+  <si>
+    <t>Prevent Code Injection</t>
+  </si>
+  <si>
+    <t>Jegliche Nutzereingaben sollten unmittelbar mittels Whitelists/Sandbox überprüft werden</t>
+  </si>
+  <si>
+    <t>JCG-008</t>
+  </si>
+  <si>
+    <t>Prevent XPath injection</t>
+  </si>
+  <si>
+    <t>XML-Input via Whitelists/Patternmatcher überprüfen</t>
+  </si>
+  <si>
+    <t>JCG-009</t>
+  </si>
+  <si>
+    <t>Prevent LDAP injection</t>
+  </si>
+  <si>
+    <t>Eingabe von Zeichen die für LDAP benutzt werden abfangen</t>
+  </si>
+  <si>
+    <t>JCG-010</t>
+  </si>
+  <si>
+    <t>Do not use the clone() method to copy untrusted method parameters</t>
+  </si>
+  <si>
+    <t>Parameter nicht mittels clone() kopieren</t>
+  </si>
+  <si>
+    <t>JCG-011</t>
+  </si>
+  <si>
+    <t>Do not use Object.equals() to compare cryptographic keys</t>
+  </si>
+  <si>
+    <t>Kryptographische Schlüssel nicht mittels equals() vergleichen</t>
+  </si>
+  <si>
+    <t>JCG-012</t>
+  </si>
+  <si>
+    <t>Do not use insecure or weak cryptographic algorithms</t>
+  </si>
+  <si>
+    <t>Keine als unsicher eingestuften Verschlüsselungsalgorithmen verwenden</t>
+  </si>
+  <si>
+    <t>JCG-013</t>
+  </si>
+  <si>
+    <t>Store passwords using a hash function</t>
+  </si>
+  <si>
+    <t>Passwörter sollten mittels Hash-Funktion als byte-array abgespeichert werden</t>
+  </si>
+  <si>
+    <t>JCG-014</t>
+  </si>
+  <si>
+    <t>Ensure that SecureRandom is properly seeded</t>
+  </si>
+  <si>
+    <t>Für SecureRandem den parameterlosen Konstruktor verwenden</t>
+  </si>
+  <si>
+    <t>JCG-015</t>
+  </si>
+  <si>
+    <t>Do not rely on methods that can be overridden by untrusted code</t>
+  </si>
+  <si>
+    <t>Standardmethoden wie equals(), clone(), hashCode(), ... nur von final-Klassen verwenden</t>
+  </si>
+  <si>
+    <t>Security, Inheritance</t>
+  </si>
+  <si>
+    <t>JCG-016</t>
+  </si>
+  <si>
+    <t>Avoid granting excess privileges</t>
+  </si>
+  <si>
+    <t>Aufruf von doPrivileged() vermeiden</t>
+  </si>
+  <si>
+    <t>JCG-017</t>
+  </si>
+  <si>
+    <t>Minimize privileged code</t>
+  </si>
+  <si>
+    <t>Aufrufe von doPrivileged() so klein wie möglich halten</t>
+  </si>
+  <si>
+    <t>JCG-018</t>
+  </si>
+  <si>
+    <t>Do not expose methods that use reduced-security checks to untrusted code</t>
+  </si>
+  <si>
+    <t>Methodenaufrufe von methoden mit reduziertem Sicherheitscheck müssen gesichert werden</t>
+  </si>
+  <si>
+    <t>JCG-019</t>
+  </si>
+  <si>
+    <t>Define custom security permissions for fine-grained security</t>
+  </si>
+  <si>
+    <t>Spezielle Berechtigungen definieren</t>
+  </si>
+  <si>
+    <t>JCG-020</t>
+  </si>
+  <si>
+    <t>Create a secure sandbox using a security manager</t>
+  </si>
+  <si>
+    <t>SecurityManager verwenden</t>
+  </si>
+  <si>
+    <t>JCG-021</t>
+  </si>
+  <si>
+    <t>Do not let untrusted code misuse privileges of callback methods</t>
+  </si>
+  <si>
+    <t>Callback sollten keine Daten von unsicherem Code akzeptieren</t>
+  </si>
+  <si>
+    <t>JCG-022</t>
+  </si>
+  <si>
+    <t>Defensive</t>
+  </si>
+  <si>
+    <t>Minimize the scope of variables</t>
+  </si>
+  <si>
+    <t>Der Geltungsbereich von Variablen sollte so klein wie möglich sein</t>
+  </si>
+  <si>
+    <t>JCG-023</t>
+  </si>
+  <si>
+    <t>Minimize the scope of the @SuppressWarnings annotation</t>
+  </si>
+  <si>
+    <t>Die SuppressWarnings-Annotation sollte möglichst nah am Code stehen, dessen Warnungen ignoriert werden sollen</t>
+  </si>
+  <si>
+    <t>Annotations</t>
+  </si>
+  <si>
+    <t>JCG-024</t>
+  </si>
+  <si>
+    <t>Minimize the accessibility of classes and their members</t>
+  </si>
+  <si>
+    <t>Die Sichtbarkeit aller Konstrukte sollte so gering wie möglich sein</t>
+  </si>
+  <si>
+    <t>JCG-025</t>
+  </si>
+  <si>
+    <t>Document thread-safety and use annotations where applicable</t>
+  </si>
+  <si>
+    <t>Beabsichtigte Thread-Sicherheit dokumentieren, wenn möglich mittels Annotationen</t>
+  </si>
+  <si>
+    <t>Concurrency, Annotations</t>
+  </si>
+  <si>
+    <t>JCG-026</t>
+  </si>
+  <si>
+    <t>Always provide feedback about the resulting value of a method</t>
+  </si>
+  <si>
+    <t>Methoden sollten Status anzeigende Rückgabewerte liefern, oder Exceptions werfen</t>
+  </si>
+  <si>
+    <t>Methods, Exceptions</t>
+  </si>
+  <si>
+    <t>JCG-027</t>
+  </si>
+  <si>
+    <t>Identify files using multiple file attributes</t>
+  </si>
+  <si>
+    <t>Bei Dateizugriff mehrere Identitäts-attribute prüfen</t>
+  </si>
+  <si>
+    <t>InOut</t>
+  </si>
+  <si>
+    <t>JCG-028</t>
+  </si>
+  <si>
+    <t>Do not attach significance to the ordinal associated with an enum</t>
+  </si>
+  <si>
+    <t>Der ordinal() Methode von Enums sollte keine implizite Bedeutung zugewiesen werden</t>
+  </si>
+  <si>
+    <t>JCG-029</t>
+  </si>
+  <si>
+    <t>Be aware of numeric promotion behavior</t>
+  </si>
+  <si>
+    <t>Implizites Casting bei Mischung von Datentypen in mathematischen Formeln beachten</t>
+  </si>
+  <si>
+    <t>Datatypes, Operators</t>
+  </si>
+  <si>
+    <t>JCG-030</t>
+  </si>
+  <si>
+    <t>Enable compile-time type checking of variable arity parameter types</t>
+  </si>
+  <si>
+    <t>Für variable Parameterlisten speziellst möglichen typ angeben</t>
+  </si>
+  <si>
+    <t>Methods, Datatypes</t>
+  </si>
+  <si>
+    <t>JCG-031</t>
+  </si>
+  <si>
+    <t>Do not apply public final to constants whose value might change in later releases</t>
+  </si>
+  <si>
+    <t>Konstanten die sich ändern könnten sollten nicht public final deklariert werden</t>
+  </si>
+  <si>
+    <t>NONAUTOMATIC</t>
+  </si>
+  <si>
+    <t>JCG-032</t>
+  </si>
+  <si>
+    <t>Avoid cyclic dependencies between packages</t>
+  </si>
+  <si>
+    <t>Packages sollten nicht gegenseitig voneinander abhängen</t>
+  </si>
+  <si>
+    <t>JCG-033</t>
+  </si>
+  <si>
+    <t>Prefer user-defined exceptions over more general exception types</t>
+  </si>
+  <si>
+    <t>Möglichst eigene Exception-Typen verwenden</t>
+  </si>
+  <si>
+    <t>JCG-034</t>
+  </si>
+  <si>
+    <t>Try to gracefully recover from system errors</t>
+  </si>
+  <si>
+    <t>Finally Blöcke und Try-With-Resources verwenden um Systemfehlern zu begegnen</t>
+  </si>
+  <si>
+    <t>JCG-035</t>
+  </si>
+  <si>
+    <t>Carefully design interfaces before releasing them</t>
+  </si>
+  <si>
+    <t>Interfaces nach veröffentlichung nicht mehr ändern - Erbende Interfaces</t>
+  </si>
+  <si>
+    <t>Inheritance, Coding</t>
+  </si>
+  <si>
+    <t>JCG-036</t>
+  </si>
+  <si>
+    <t>Write garbage collection-firendly code</t>
+  </si>
+  <si>
+    <t>Immutable Objekte mit kurzer Lebensdauer, möglichst keine großen Objekte und keine expliziten Aufrufe des Garbage Collectors verwenden</t>
+  </si>
+  <si>
+    <t>JCG-037</t>
+  </si>
+  <si>
+    <t>Reliability</t>
+  </si>
+  <si>
+    <t>Do not shadow or obscure identifiers in subscopes</t>
+  </si>
+  <si>
+    <t>Bezeichner sollten nicht im gleichen Geltungsbereich Überdeckt werden</t>
+  </si>
+  <si>
+    <t>JCG-038</t>
+  </si>
+  <si>
+    <t>Do not declare more than one variable per declaration</t>
+  </si>
+  <si>
+    <t>Pro Deklarationsanweisung sollte nur eine Variable deklariert werden</t>
+  </si>
+  <si>
+    <t>JCG-039</t>
+  </si>
+  <si>
+    <t>Use meaningful symbolic constants to represent literal values in program logic</t>
+  </si>
+  <si>
+    <t>Literale sollten als Konstante Klassenvariablen deklariert werden</t>
+  </si>
+  <si>
+    <t>JCG-040</t>
+  </si>
+  <si>
+    <t>Properly encode relationships in constant definitions</t>
+  </si>
+  <si>
+    <t>Konstanten sollten nur voneinander Abhängen, wenn die Bedeutung auch voneinander abhängt</t>
+  </si>
+  <si>
+    <t>JCG-041</t>
+  </si>
+  <si>
+    <t>Return an empty array or collection instead of a null value for methods that return an array or collection</t>
+  </si>
+  <si>
+    <t>Methoden sollten leere Arrays / Collections zurückgeben anstatt null</t>
+  </si>
+  <si>
+    <t>Methods, Collections</t>
+  </si>
+  <si>
+    <t>JCG-042</t>
+  </si>
+  <si>
+    <t>Use exceptions only for exceptionel conditions</t>
+  </si>
+  <si>
+    <t>Exceptions sollten nur für Fehler verwendet werden, nicht für normalen Kontrollfluss</t>
+  </si>
+  <si>
+    <t>JCG-043</t>
+  </si>
+  <si>
+    <t>Use a try-with-resources statement to safely handle closeable resources</t>
+  </si>
+  <si>
+    <t>Für alle Resourcen die Closable implementieren try-with-resources verwenden</t>
+  </si>
+  <si>
+    <t>Exceptions, InOut</t>
+  </si>
+  <si>
+    <t>JCG-044</t>
+  </si>
+  <si>
+    <t>Do not use assertions to verify the absence of runtime errors</t>
+  </si>
+  <si>
+    <t>Runtime Exceptions dürfen nicht mit assertions überprüft werden</t>
+  </si>
+  <si>
+    <t>Exceptions, Assertions</t>
+  </si>
+  <si>
+    <t>JCG-045</t>
+  </si>
+  <si>
+    <t>Use the same type for the second and third operands in conditional expressions</t>
+  </si>
+  <si>
+    <t>Der zweite und dritte operand in conditional expressions sollten den gleichen typ haben (operand1 ? operand2 : operand3)</t>
+  </si>
+  <si>
+    <t>Conditionals, Datatypes</t>
+  </si>
+  <si>
+    <t>JCG-046</t>
+  </si>
+  <si>
+    <t>Do not serialize direct handles to system resources</t>
+  </si>
+  <si>
+    <t>Keine Systemresourcen in Serializable Klassen verwenden</t>
+  </si>
+  <si>
+    <t>JCG-047</t>
+  </si>
+  <si>
+    <t>Prefer using iterators over enumerations</t>
+  </si>
+  <si>
+    <t>Wenn möglich Iterators statt Enums verwenden</t>
+  </si>
+  <si>
+    <t>JCG-048</t>
+  </si>
+  <si>
+    <t>Do not use direct buffers for short-lived, infrequently used objects</t>
+  </si>
+  <si>
+    <t>Direct Buffers nicht für wenig / einmalig benutzte Objekte benutzen</t>
+  </si>
+  <si>
+    <t>JCG-049</t>
+  </si>
+  <si>
+    <t>Remove short-lived objects from long-lived container objects</t>
+  </si>
+  <si>
+    <t>Kurz benötigte Objekte nach verwendung aus langlebigen Containern entfernen</t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>JCG-050</t>
+  </si>
+  <si>
+    <t>Understandability</t>
+  </si>
+  <si>
+    <t>Be careful using visually misleading identifiers and literals</t>
+  </si>
+  <si>
+    <t>Verwechselbare Zeichen nicht als alleinige Bezeichner oder einzigen Unterschied zwischen Bezeichnern verwenden</t>
+  </si>
+  <si>
+    <t>JCG-051</t>
+  </si>
+  <si>
+    <t>Avoid ambiguous overloading of variable arity methods</t>
+  </si>
+  <si>
+    <t>Methoden mit variablen Parameterlisten sollten nicht überladen werden</t>
+  </si>
+  <si>
+    <t>JCG-052</t>
+  </si>
+  <si>
+    <t>Avoid in-band error indicators</t>
+  </si>
+  <si>
+    <t>Rückgabewerte sollten keine Fehler repräsentieren</t>
+  </si>
+  <si>
+    <t>JCG-053</t>
+  </si>
+  <si>
+    <t>Do not perform assignments in conditional expressions</t>
+  </si>
+  <si>
+    <t>In Bedingungen keine Wertzuweisung vornehmen</t>
+  </si>
+  <si>
+    <t>Variables, Conditionals</t>
+  </si>
+  <si>
+    <t>JCG-054</t>
+  </si>
+  <si>
+    <t>Use braces for the body of an if, for, or while statement</t>
+  </si>
+  <si>
+    <t>Für alle if, for und while anweisungen den inhalt in Klammern setzen</t>
+  </si>
+  <si>
+    <t>Conditionals, Style</t>
+  </si>
+  <si>
+    <t>JCG-055</t>
+  </si>
+  <si>
+    <t>Do not place a semicolon immediatly following an if, for or while condition</t>
+  </si>
+  <si>
+    <t>Nach Bedingungen von If, For oder While Anweisungen sollte kein Semikolon folgen</t>
+  </si>
+  <si>
+    <t>JCG-056</t>
+  </si>
+  <si>
+    <t>Finish every set of statements associated with a case label with a break statement</t>
+  </si>
+  <si>
+    <t>Case-Anweisungen sollten mit immer mit break abgeschlossen werden</t>
+  </si>
+  <si>
+    <t>JCG-057</t>
+  </si>
+  <si>
+    <t>Avoid inadvertent wrapping of loop counters</t>
+  </si>
+  <si>
+    <t>Für Schleifen keine unereichbaren oder überspringbaren Abbruchbedingungen definieren</t>
+  </si>
+  <si>
+    <t>JCG-058</t>
+  </si>
+  <si>
+    <t>Use parentheses for precedence of operation</t>
+  </si>
+  <si>
+    <t>Nicht-triviale Operationen mit Klammern gliedern</t>
+  </si>
+  <si>
+    <t>JCG-059</t>
+  </si>
+  <si>
+    <t>Do not make assumptions about file creation</t>
+  </si>
+  <si>
+    <t>Sichere Datei-erzeugung anwenden mit nio-packages</t>
+  </si>
+  <si>
+    <t>JCG-060</t>
+  </si>
+  <si>
+    <t>Convert integers to floating-point for floating-point operations</t>
+  </si>
+  <si>
+    <t>Integer vor verwendung in fließkommaoperationen in fließkommazahlen umwandeln</t>
+  </si>
+  <si>
+    <t>JCG-061</t>
+  </si>
+  <si>
+    <t>Ensure that the clone() method calls super.clone()</t>
+  </si>
+  <si>
+    <t>Alle clone() Methoden müssen super.clone() aufrufen</t>
+  </si>
+  <si>
+    <t>JCG-062</t>
+  </si>
+  <si>
+    <t>Use comments consistently and in a readable fashion</t>
+  </si>
+  <si>
+    <t>Zeilen und Block-Kommentare nicht mischen und Konsistent benutzen</t>
+  </si>
+  <si>
+    <t>JCG-063</t>
+  </si>
+  <si>
+    <t>Detect and remove superfluous code and values</t>
+  </si>
+  <si>
+    <t>Ungenutzer Code und Variablen, sowie Code ohne Effekte sollte entfernt werden</t>
+  </si>
+  <si>
+    <t>JCG-064</t>
+  </si>
+  <si>
+    <t>Strive for logical completeness</t>
+  </si>
+  <si>
+    <t>Alle möglichen Daten-Zustände sollten behandelt werden</t>
+  </si>
+  <si>
+    <t>JCG-065</t>
+  </si>
+  <si>
+    <t>Avoid ambiguous or confusing uses of overloading</t>
+  </si>
+  <si>
+    <t>Überladene Methoden die sich nur in Reihenfolge der Parametertypen unterscheiden vermeiden</t>
+  </si>
+  <si>
+    <t>JCG-066</t>
+  </si>
+  <si>
+    <t>Misconception</t>
+  </si>
+  <si>
+    <t>Do not assume that declaring a reference volatile guarantees safe publication of the referenced object</t>
+  </si>
+  <si>
+    <t>Volatile Variablendeklarationen nicht für Thread-Sicherheit verwenden</t>
+  </si>
+  <si>
+    <t>JCG-067</t>
+  </si>
+  <si>
+    <t>Do not assume that the sleep(), yield(), or getState() methods provide synchronization semantics</t>
+  </si>
+  <si>
+    <t>Die sleep(), yield() und getState() Methoden nicht für Synchronisation benutzen</t>
+  </si>
+  <si>
+    <t>JCG-068</t>
+  </si>
+  <si>
+    <t>Do not assume that the remainder operator always returns nonnegative result for integral operands</t>
+  </si>
+  <si>
+    <t>Modulo Operator (%) nicht für zwangsläufig positive Ergebnisse verwenden</t>
+  </si>
+  <si>
+    <t>JCG-069</t>
+  </si>
+  <si>
+    <t>Do not confuse abstract object equality with reference equality</t>
+  </si>
+  <si>
+    <t>== und != nicht verwenden um Objektgleichheit zu prüfen</t>
+  </si>
+  <si>
+    <t>JCG-070</t>
+  </si>
+  <si>
+    <t>Understand the difference between bitwise and logical operators</t>
+  </si>
+  <si>
+    <t>Bitweise Operatoren nicht verwenden wenn zweiter Operator nicht immer evaluiert werden soll</t>
+  </si>
+  <si>
+    <t>JCG-071</t>
+  </si>
+  <si>
+    <t>Understand how escape characters are interpreted when strings are loaded</t>
+  </si>
+  <si>
+    <t>SQL-Escapes müssen doppelt escaped werden</t>
+  </si>
+  <si>
+    <t>JCG-072</t>
+  </si>
+  <si>
+    <t>Do not use overloaded methods to differentiate between runtime types</t>
+  </si>
+  <si>
+    <t>Überladene Methoden nicht zum unterscheiden von Objekttypen benutzen</t>
+  </si>
+  <si>
+    <t>JCG-073</t>
+  </si>
+  <si>
+    <t>Never confuse the immutability of a reference with that of the referenced object</t>
+  </si>
+  <si>
+    <t>Nicht nur die Referenz final deklarieren, wenn das referenzierte Objekt unveränderbar werden soll</t>
+  </si>
+  <si>
+    <t>Variables,UNAUTOMATIC</t>
+  </si>
+  <si>
+    <t>JCG-074</t>
+  </si>
+  <si>
+    <t>Use the serialization methods writeUnshared() and readUnshared() with care</t>
+  </si>
+  <si>
+    <t>Die writeUnshared() und readUnshared() Methoden nicht für round-trip-serialisierung verwenden</t>
+  </si>
+  <si>
+    <t>Concurrency, Methods</t>
+  </si>
+  <si>
+    <t>JCG-075</t>
+  </si>
+  <si>
+    <t>Do not attempt to help the garbage collector by setting local reference variables to null</t>
+  </si>
+  <si>
+    <t>Referenzvariablen nicht auf null setzen wenn sie nicht mehr gebraucht werden</t>
+  </si>
+  <si>
+    <t>SPD-001</t>
+  </si>
+  <si>
+    <t>Java Naming Conventions</t>
+  </si>
+  <si>
+    <t>Für alle Bezeichner Java Namenskonventionen einhalten</t>
+  </si>
+  <si>
+    <t>SPD-002</t>
+  </si>
+  <si>
+    <t>Meaningful Names</t>
+  </si>
+  <si>
+    <t>Alle Bezeichner mindestens 4 Zeichen lang und sprechend</t>
+  </si>
+  <si>
+    <t>SPD-003</t>
+  </si>
+  <si>
+    <t>Maximale Methodenlänge von 40 Zeilen nicht überschreiten</t>
+  </si>
+  <si>
+    <t>SPD-004</t>
+  </si>
+  <si>
+    <t>Parameterlist length</t>
+  </si>
+  <si>
+    <t>Maximal 5 Parameter in Methodensignatur</t>
+  </si>
+  <si>
+    <t>SPD-005</t>
+  </si>
+  <si>
+    <t>Cyclomatic Complexity</t>
+  </si>
+  <si>
+    <t>McCabe-Komplexität jeder Methode sollte höchstens 10 sein</t>
+  </si>
+  <si>
+    <t>SPD-006</t>
+  </si>
+  <si>
+    <t>Klassen sollten höchstens 400 Zeilen lang sein</t>
+  </si>
+  <si>
+    <t>SPD-007</t>
+  </si>
+  <si>
+    <t>Dead Code</t>
+  </si>
+  <si>
+    <t>Ungenutzer Code sollte entfernt werden</t>
+  </si>
+  <si>
+    <t>Classes, Unused</t>
+  </si>
+  <si>
+    <t>SPD-008</t>
+  </si>
+  <si>
+    <t>Godclass</t>
+  </si>
+  <si>
+    <t>Summe aller Methodenkomplexitäten (WMC) &lt; 48, Zugriffe auf Variablen anderer Klassen (AFTD) &lt; 6, Anteil über Variablenzugriffe zusammenhängende Methoden (TCC) &gt; 0,32</t>
+  </si>
+  <si>
+    <t>SPD-009</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Literals</t>
+  </si>
+  <si>
+    <t>Keine Verwendung von Literalen im Code - Konstanten</t>
+  </si>
+  <si>
+    <t>SPD-010</t>
+  </si>
+  <si>
+    <t>Deeply nested if statements</t>
+  </si>
+  <si>
+    <t>Maximale Verschachtelungstiefe von If Anweisungen = 3</t>
+  </si>
+  <si>
+    <t>SPD-011</t>
+  </si>
+  <si>
+    <t>Field declaration</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Method length</t>
+  </si>
+  <si>
+    <t>Class length</t>
   </si>
 </sst>
 </file>
@@ -2435,6 +3317,14 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Ruleset_Code-Quality-Index" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Ruleset_Java-Coding-Guidelines" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Ruleset_Softwarepraktikum-Dortmund" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7365,12 +8255,1797 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A53" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B2" t="s">
+        <v>771</v>
+      </c>
+      <c r="C2" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2" t="s">
+        <v>773</v>
+      </c>
+      <c r="E2" t="s">
+        <v>771</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B3" t="s">
+        <v>771</v>
+      </c>
+      <c r="C3" t="s">
+        <v>775</v>
+      </c>
+      <c r="D3" t="s">
+        <v>776</v>
+      </c>
+      <c r="E3" t="s">
+        <v>771</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B4" t="s">
+        <v>771</v>
+      </c>
+      <c r="C4" t="s">
+        <v>778</v>
+      </c>
+      <c r="D4" t="s">
+        <v>779</v>
+      </c>
+      <c r="E4" t="s">
+        <v>771</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B5" t="s">
+        <v>771</v>
+      </c>
+      <c r="C5" t="s">
+        <v>781</v>
+      </c>
+      <c r="D5" t="s">
+        <v>782</v>
+      </c>
+      <c r="E5" t="s">
+        <v>783</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B6" t="s">
+        <v>771</v>
+      </c>
+      <c r="C6" t="s">
+        <v>785</v>
+      </c>
+      <c r="D6" t="s">
+        <v>786</v>
+      </c>
+      <c r="E6" t="s">
+        <v>787</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B7" t="s">
+        <v>771</v>
+      </c>
+      <c r="C7" t="s">
+        <v>789</v>
+      </c>
+      <c r="D7" t="s">
+        <v>790</v>
+      </c>
+      <c r="E7" t="s">
+        <v>787</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B8" t="s">
+        <v>771</v>
+      </c>
+      <c r="C8" t="s">
+        <v>792</v>
+      </c>
+      <c r="D8" t="s">
+        <v>793</v>
+      </c>
+      <c r="E8" t="s">
+        <v>787</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B9" t="s">
+        <v>771</v>
+      </c>
+      <c r="C9" t="s">
+        <v>795</v>
+      </c>
+      <c r="D9" t="s">
+        <v>796</v>
+      </c>
+      <c r="E9" t="s">
+        <v>787</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B10" t="s">
+        <v>771</v>
+      </c>
+      <c r="C10" t="s">
+        <v>798</v>
+      </c>
+      <c r="D10" t="s">
+        <v>799</v>
+      </c>
+      <c r="E10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="B11" t="s">
+        <v>771</v>
+      </c>
+      <c r="C11" t="s">
+        <v>801</v>
+      </c>
+      <c r="D11" t="s">
+        <v>802</v>
+      </c>
+      <c r="E11" t="s">
+        <v>783</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B12" t="s">
+        <v>771</v>
+      </c>
+      <c r="C12" t="s">
+        <v>804</v>
+      </c>
+      <c r="D12" t="s">
+        <v>805</v>
+      </c>
+      <c r="E12" t="s">
+        <v>771</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B13" t="s">
+        <v>771</v>
+      </c>
+      <c r="C13" t="s">
+        <v>807</v>
+      </c>
+      <c r="D13" t="s">
+        <v>808</v>
+      </c>
+      <c r="E13" t="s">
+        <v>771</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B14" t="s">
+        <v>771</v>
+      </c>
+      <c r="C14" t="s">
+        <v>810</v>
+      </c>
+      <c r="D14" t="s">
+        <v>811</v>
+      </c>
+      <c r="E14" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B15" t="s">
+        <v>771</v>
+      </c>
+      <c r="C15" t="s">
+        <v>813</v>
+      </c>
+      <c r="D15" t="s">
+        <v>814</v>
+      </c>
+      <c r="E15" t="s">
+        <v>771</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B16" t="s">
+        <v>771</v>
+      </c>
+      <c r="C16" t="s">
+        <v>816</v>
+      </c>
+      <c r="D16" t="s">
+        <v>817</v>
+      </c>
+      <c r="E16" t="s">
+        <v>818</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="B17" t="s">
+        <v>771</v>
+      </c>
+      <c r="C17" t="s">
+        <v>820</v>
+      </c>
+      <c r="D17" t="s">
+        <v>821</v>
+      </c>
+      <c r="E17" t="s">
+        <v>771</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B18" t="s">
+        <v>771</v>
+      </c>
+      <c r="C18" t="s">
+        <v>823</v>
+      </c>
+      <c r="D18" t="s">
+        <v>824</v>
+      </c>
+      <c r="E18" t="s">
+        <v>771</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B19" t="s">
+        <v>771</v>
+      </c>
+      <c r="C19" t="s">
+        <v>826</v>
+      </c>
+      <c r="D19" t="s">
+        <v>827</v>
+      </c>
+      <c r="E19" t="s">
+        <v>771</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B20" t="s">
+        <v>771</v>
+      </c>
+      <c r="C20" t="s">
+        <v>829</v>
+      </c>
+      <c r="D20" t="s">
+        <v>830</v>
+      </c>
+      <c r="E20" t="s">
+        <v>771</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="B21" t="s">
+        <v>771</v>
+      </c>
+      <c r="C21" t="s">
+        <v>832</v>
+      </c>
+      <c r="D21" t="s">
+        <v>833</v>
+      </c>
+      <c r="E21" t="s">
+        <v>771</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="B22" t="s">
+        <v>771</v>
+      </c>
+      <c r="C22" t="s">
+        <v>835</v>
+      </c>
+      <c r="D22" t="s">
+        <v>836</v>
+      </c>
+      <c r="E22" t="s">
+        <v>771</v>
+      </c>
+      <c r="F22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="B23" t="s">
+        <v>838</v>
+      </c>
+      <c r="C23" t="s">
+        <v>839</v>
+      </c>
+      <c r="D23" t="s">
+        <v>840</v>
+      </c>
+      <c r="E23" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="B24" t="s">
+        <v>838</v>
+      </c>
+      <c r="C24" t="s">
+        <v>842</v>
+      </c>
+      <c r="D24" t="s">
+        <v>843</v>
+      </c>
+      <c r="E24" t="s">
+        <v>844</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="B25" t="s">
+        <v>838</v>
+      </c>
+      <c r="C25" t="s">
+        <v>846</v>
+      </c>
+      <c r="D25" t="s">
+        <v>847</v>
+      </c>
+      <c r="E25" t="s">
+        <v>436</v>
+      </c>
+      <c r="F25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="B26" t="s">
+        <v>838</v>
+      </c>
+      <c r="C26" t="s">
+        <v>849</v>
+      </c>
+      <c r="D26" t="s">
+        <v>850</v>
+      </c>
+      <c r="E26" t="s">
+        <v>851</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="B27" t="s">
+        <v>838</v>
+      </c>
+      <c r="C27" t="s">
+        <v>853</v>
+      </c>
+      <c r="D27" t="s">
+        <v>854</v>
+      </c>
+      <c r="E27" t="s">
+        <v>855</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="B28" t="s">
+        <v>838</v>
+      </c>
+      <c r="C28" t="s">
+        <v>857</v>
+      </c>
+      <c r="D28" t="s">
+        <v>858</v>
+      </c>
+      <c r="E28" t="s">
+        <v>859</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B29" t="s">
+        <v>838</v>
+      </c>
+      <c r="C29" t="s">
+        <v>861</v>
+      </c>
+      <c r="D29" t="s">
+        <v>862</v>
+      </c>
+      <c r="E29" t="s">
+        <v>547</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B30" t="s">
+        <v>838</v>
+      </c>
+      <c r="C30" t="s">
+        <v>864</v>
+      </c>
+      <c r="D30" t="s">
+        <v>865</v>
+      </c>
+      <c r="E30" t="s">
+        <v>866</v>
+      </c>
+      <c r="F30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="B31" t="s">
+        <v>838</v>
+      </c>
+      <c r="C31" t="s">
+        <v>868</v>
+      </c>
+      <c r="D31" t="s">
+        <v>869</v>
+      </c>
+      <c r="E31" t="s">
+        <v>870</v>
+      </c>
+      <c r="F31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="B32" t="s">
+        <v>838</v>
+      </c>
+      <c r="C32" t="s">
+        <v>872</v>
+      </c>
+      <c r="D32" t="s">
+        <v>873</v>
+      </c>
+      <c r="E32" t="s">
+        <v>498</v>
+      </c>
+      <c r="F32" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="B33" t="s">
+        <v>838</v>
+      </c>
+      <c r="C33" t="s">
+        <v>876</v>
+      </c>
+      <c r="D33" t="s">
+        <v>877</v>
+      </c>
+      <c r="E33" t="s">
+        <v>362</v>
+      </c>
+      <c r="F33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="B34" t="s">
+        <v>838</v>
+      </c>
+      <c r="C34" t="s">
+        <v>879</v>
+      </c>
+      <c r="D34" t="s">
+        <v>880</v>
+      </c>
+      <c r="E34" t="s">
+        <v>291</v>
+      </c>
+      <c r="F34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B35" t="s">
+        <v>838</v>
+      </c>
+      <c r="C35" t="s">
+        <v>882</v>
+      </c>
+      <c r="D35" t="s">
+        <v>883</v>
+      </c>
+      <c r="E35" t="s">
+        <v>291</v>
+      </c>
+      <c r="F35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="B36" t="s">
+        <v>838</v>
+      </c>
+      <c r="C36" t="s">
+        <v>885</v>
+      </c>
+      <c r="D36" t="s">
+        <v>886</v>
+      </c>
+      <c r="E36" t="s">
+        <v>887</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B37" t="s">
+        <v>838</v>
+      </c>
+      <c r="C37" t="s">
+        <v>889</v>
+      </c>
+      <c r="D37" t="s">
+        <v>890</v>
+      </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="B38" t="s">
+        <v>892</v>
+      </c>
+      <c r="C38" t="s">
+        <v>893</v>
+      </c>
+      <c r="D38" t="s">
+        <v>894</v>
+      </c>
+      <c r="E38" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="B39" t="s">
+        <v>892</v>
+      </c>
+      <c r="C39" t="s">
+        <v>896</v>
+      </c>
+      <c r="D39" t="s">
+        <v>897</v>
+      </c>
+      <c r="E39" t="s">
+        <v>108</v>
+      </c>
+      <c r="F39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B40" t="s">
+        <v>892</v>
+      </c>
+      <c r="C40" t="s">
+        <v>899</v>
+      </c>
+      <c r="D40" t="s">
+        <v>900</v>
+      </c>
+      <c r="E40" t="s">
+        <v>531</v>
+      </c>
+      <c r="F40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B41" t="s">
+        <v>892</v>
+      </c>
+      <c r="C41" t="s">
+        <v>902</v>
+      </c>
+      <c r="D41" t="s">
+        <v>903</v>
+      </c>
+      <c r="E41" t="s">
+        <v>498</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B42" t="s">
+        <v>892</v>
+      </c>
+      <c r="C42" t="s">
+        <v>905</v>
+      </c>
+      <c r="D42" t="s">
+        <v>906</v>
+      </c>
+      <c r="E42" t="s">
+        <v>907</v>
+      </c>
+      <c r="F42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="B43" t="s">
+        <v>892</v>
+      </c>
+      <c r="C43" t="s">
+        <v>909</v>
+      </c>
+      <c r="D43" t="s">
+        <v>910</v>
+      </c>
+      <c r="E43" t="s">
+        <v>291</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="B44" t="s">
+        <v>892</v>
+      </c>
+      <c r="C44" t="s">
+        <v>912</v>
+      </c>
+      <c r="D44" t="s">
+        <v>913</v>
+      </c>
+      <c r="E44" t="s">
+        <v>914</v>
+      </c>
+      <c r="F44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="B45" t="s">
+        <v>892</v>
+      </c>
+      <c r="C45" t="s">
+        <v>916</v>
+      </c>
+      <c r="D45" t="s">
+        <v>917</v>
+      </c>
+      <c r="E45" t="s">
+        <v>918</v>
+      </c>
+      <c r="F45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="B46" t="s">
+        <v>892</v>
+      </c>
+      <c r="C46" t="s">
+        <v>920</v>
+      </c>
+      <c r="D46" t="s">
+        <v>921</v>
+      </c>
+      <c r="E46" t="s">
+        <v>922</v>
+      </c>
+      <c r="F46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="B47" t="s">
+        <v>892</v>
+      </c>
+      <c r="C47" t="s">
+        <v>924</v>
+      </c>
+      <c r="D47" t="s">
+        <v>925</v>
+      </c>
+      <c r="E47" t="s">
+        <v>859</v>
+      </c>
+      <c r="F47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="B48" t="s">
+        <v>892</v>
+      </c>
+      <c r="C48" t="s">
+        <v>927</v>
+      </c>
+      <c r="D48" t="s">
+        <v>928</v>
+      </c>
+      <c r="E48" t="s">
+        <v>547</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="B49" t="s">
+        <v>892</v>
+      </c>
+      <c r="C49" t="s">
+        <v>930</v>
+      </c>
+      <c r="D49" t="s">
+        <v>931</v>
+      </c>
+      <c r="E49" t="s">
+        <v>671</v>
+      </c>
+      <c r="F49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B50" t="s">
+        <v>892</v>
+      </c>
+      <c r="C50" t="s">
+        <v>933</v>
+      </c>
+      <c r="D50" t="s">
+        <v>934</v>
+      </c>
+      <c r="E50" t="s">
+        <v>935</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="B51" t="s">
+        <v>937</v>
+      </c>
+      <c r="C51" t="s">
+        <v>938</v>
+      </c>
+      <c r="D51" t="s">
+        <v>939</v>
+      </c>
+      <c r="E51" t="s">
+        <v>39</v>
+      </c>
+      <c r="F51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="B52" t="s">
+        <v>937</v>
+      </c>
+      <c r="C52" t="s">
+        <v>941</v>
+      </c>
+      <c r="D52" t="s">
+        <v>942</v>
+      </c>
+      <c r="E52" t="s">
+        <v>264</v>
+      </c>
+      <c r="F52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="B53" t="s">
+        <v>937</v>
+      </c>
+      <c r="C53" t="s">
+        <v>944</v>
+      </c>
+      <c r="D53" t="s">
+        <v>945</v>
+      </c>
+      <c r="E53" t="s">
+        <v>291</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="B54" t="s">
+        <v>937</v>
+      </c>
+      <c r="C54" t="s">
+        <v>947</v>
+      </c>
+      <c r="D54" t="s">
+        <v>948</v>
+      </c>
+      <c r="E54" t="s">
+        <v>949</v>
+      </c>
+      <c r="F54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="B55" t="s">
+        <v>937</v>
+      </c>
+      <c r="C55" t="s">
+        <v>951</v>
+      </c>
+      <c r="D55" t="s">
+        <v>952</v>
+      </c>
+      <c r="E55" t="s">
+        <v>953</v>
+      </c>
+      <c r="F55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="B56" t="s">
+        <v>937</v>
+      </c>
+      <c r="C56" t="s">
+        <v>955</v>
+      </c>
+      <c r="D56" t="s">
+        <v>956</v>
+      </c>
+      <c r="E56" t="s">
+        <v>953</v>
+      </c>
+      <c r="F56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="B57" t="s">
+        <v>937</v>
+      </c>
+      <c r="C57" t="s">
+        <v>958</v>
+      </c>
+      <c r="D57" t="s">
+        <v>959</v>
+      </c>
+      <c r="E57" t="s">
+        <v>268</v>
+      </c>
+      <c r="F57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="B58" t="s">
+        <v>937</v>
+      </c>
+      <c r="C58" t="s">
+        <v>961</v>
+      </c>
+      <c r="D58" t="s">
+        <v>962</v>
+      </c>
+      <c r="E58" t="s">
+        <v>268</v>
+      </c>
+      <c r="F58" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="B59" t="s">
+        <v>937</v>
+      </c>
+      <c r="C59" t="s">
+        <v>964</v>
+      </c>
+      <c r="D59" t="s">
+        <v>965</v>
+      </c>
+      <c r="E59" t="s">
+        <v>272</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="B60" t="s">
+        <v>937</v>
+      </c>
+      <c r="C60" t="s">
+        <v>967</v>
+      </c>
+      <c r="D60" t="s">
+        <v>968</v>
+      </c>
+      <c r="E60" t="s">
+        <v>859</v>
+      </c>
+      <c r="F60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="B61" t="s">
+        <v>937</v>
+      </c>
+      <c r="C61" t="s">
+        <v>970</v>
+      </c>
+      <c r="D61" t="s">
+        <v>971</v>
+      </c>
+      <c r="E61" t="s">
+        <v>236</v>
+      </c>
+      <c r="F61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="B62" t="s">
+        <v>937</v>
+      </c>
+      <c r="C62" t="s">
+        <v>973</v>
+      </c>
+      <c r="D62" t="s">
+        <v>974</v>
+      </c>
+      <c r="E62" t="s">
+        <v>244</v>
+      </c>
+      <c r="F62" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="B63" t="s">
+        <v>937</v>
+      </c>
+      <c r="C63" t="s">
+        <v>976</v>
+      </c>
+      <c r="D63" t="s">
+        <v>977</v>
+      </c>
+      <c r="E63" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="B64" t="s">
+        <v>937</v>
+      </c>
+      <c r="C64" t="s">
+        <v>979</v>
+      </c>
+      <c r="D64" t="s">
+        <v>980</v>
+      </c>
+      <c r="E64" t="s">
+        <v>734</v>
+      </c>
+      <c r="F64" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="B65" t="s">
+        <v>937</v>
+      </c>
+      <c r="C65" t="s">
+        <v>982</v>
+      </c>
+      <c r="D65" t="s">
+        <v>983</v>
+      </c>
+      <c r="E65" t="s">
+        <v>681</v>
+      </c>
+      <c r="F65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="B66" t="s">
+        <v>937</v>
+      </c>
+      <c r="C66" t="s">
+        <v>985</v>
+      </c>
+      <c r="D66" t="s">
+        <v>986</v>
+      </c>
+      <c r="E66" t="s">
+        <v>264</v>
+      </c>
+      <c r="F66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="B67" t="s">
+        <v>988</v>
+      </c>
+      <c r="C67" t="s">
+        <v>989</v>
+      </c>
+      <c r="D67" t="s">
+        <v>990</v>
+      </c>
+      <c r="E67" t="s">
+        <v>325</v>
+      </c>
+      <c r="F67" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="B68" t="s">
+        <v>988</v>
+      </c>
+      <c r="C68" t="s">
+        <v>992</v>
+      </c>
+      <c r="D68" t="s">
+        <v>993</v>
+      </c>
+      <c r="E68" t="s">
+        <v>325</v>
+      </c>
+      <c r="F68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="B69" t="s">
+        <v>988</v>
+      </c>
+      <c r="C69" t="s">
+        <v>995</v>
+      </c>
+      <c r="D69" t="s">
+        <v>996</v>
+      </c>
+      <c r="E69" t="s">
+        <v>272</v>
+      </c>
+      <c r="F69" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="B70" t="s">
+        <v>988</v>
+      </c>
+      <c r="C70" t="s">
+        <v>998</v>
+      </c>
+      <c r="D70" t="s">
+        <v>999</v>
+      </c>
+      <c r="E70" t="s">
+        <v>272</v>
+      </c>
+      <c r="F70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B71" t="s">
+        <v>988</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E71" t="s">
+        <v>272</v>
+      </c>
+      <c r="F71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B72" t="s">
+        <v>988</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E72" t="s">
+        <v>236</v>
+      </c>
+      <c r="F72" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B73" t="s">
+        <v>988</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E73" t="s">
+        <v>264</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B74" t="s">
+        <v>988</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B75" t="s">
+        <v>988</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B76" t="s">
+        <v>988</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E76" t="s">
+        <v>108</v>
+      </c>
+      <c r="F76" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B7" t="s">
+        <v>671</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E7" t="s">
+        <v>671</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B8" t="s">
+        <v>671</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B9" t="s">
+        <v>671</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E9" t="s">
+        <v>671</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E10" t="s">
+        <v>498</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E11" t="s">
+        <v>268</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>